<commit_message>
ajustes a documento -alcance-ajustes de prueba
</commit_message>
<xml_diff>
--- a/ESTRATEGIA(PROCESO DE PRUEBAS).xlsx
+++ b/ESTRATEGIA(PROCESO DE PRUEBAS).xlsx
@@ -3,19 +3,19 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26216"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="1395" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DE15BF48-C75C-40F1-AD5A-523E8272CC57}"/>
+  <xr:revisionPtr revIDLastSave="1560" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3367A073-DDAD-49BE-9600-D8DB02DF0751}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VISIÓN" sheetId="3" r:id="rId1"/>
     <sheet name="HISTORIA DE USUARIO" sheetId="1" r:id="rId2"/>
-    <sheet name="ESTIMACIÓN" sheetId="2" r:id="rId3"/>
+    <sheet name="ESTIMACION" sheetId="2" r:id="rId3"/>
     <sheet name="RIESGOS" sheetId="4" r:id="rId4"/>
     <sheet name="PLANEACIÓN" sheetId="6" r:id="rId5"/>
     <sheet name="CASOS DE PRUEBA" sheetId="5" r:id="rId6"/>
     <sheet name="CAMINO (NO) FELIZ " sheetId="7" r:id="rId7"/>
-    <sheet name="Hoja1" sheetId="8" r:id="rId8"/>
+    <sheet name="GESTIÓN RIESGOS" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="249">
   <si>
     <t xml:space="preserve">Check List </t>
   </si>
@@ -242,122 +242,671 @@
 5- Una vez se logren visualizar los cursos disponibles, se debe poder visualizar en cada curso información previa como Titulo del Curso, Categoría y Profesor del curso. </t>
   </si>
   <si>
-    <t>Actividades</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Frecuencia </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Esfuerzo Unidad </t>
-  </si>
-  <si>
-    <t>Esfuerzo total</t>
-  </si>
-  <si>
-    <t>Visión</t>
-  </si>
-  <si>
-    <t>Reunión de entendimiento</t>
-  </si>
-  <si>
-    <t>Plan de pruebas general</t>
-  </si>
-  <si>
-    <t>Logistica</t>
-  </si>
-  <si>
-    <t>Asignación de rol analistas</t>
-  </si>
-  <si>
-    <t>Ceremonias SCRUM</t>
-  </si>
-  <si>
-    <t>Planteamiento Herramienta de pruebas</t>
-  </si>
-  <si>
-    <t>Verificación de datos</t>
-  </si>
-  <si>
-    <t>Preparacion ambientes</t>
-  </si>
-  <si>
-    <t>Planeacion</t>
-  </si>
-  <si>
-    <t>Cronograma de actividades</t>
-  </si>
-  <si>
-    <t>Plan detallado de pruebas
- Analistas: 3</t>
-  </si>
-  <si>
-    <t>Reunion aprobacion</t>
-  </si>
-  <si>
-    <t>Diseño</t>
-  </si>
-  <si>
-    <t>Pruebas funcionales - Riesgos</t>
-  </si>
-  <si>
-    <t>Pruebas de Usabilidad - Riesgos</t>
-  </si>
-  <si>
-    <t>Pruebas de Rendimiento - Riesgos</t>
-  </si>
-  <si>
-    <t>Ejecución</t>
-  </si>
-  <si>
-    <t>Pruebas exploratorias</t>
-  </si>
-  <si>
-    <t>Partición de equivalencia</t>
-  </si>
-  <si>
-    <t>Transición de Estados</t>
-  </si>
-  <si>
-    <t>Usabilidad</t>
-  </si>
-  <si>
-    <t>Pruebas de Rendimiento</t>
-  </si>
-  <si>
-    <t>Reporte de issues</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gestión </t>
-  </si>
-  <si>
-    <t>Gestión de issues</t>
-  </si>
-  <si>
-    <t>Entrega de prueba</t>
-  </si>
-  <si>
-    <t>Informe resultados pruebas</t>
-  </si>
-  <si>
-    <t>Esfuerzo estimado</t>
-  </si>
-  <si>
-    <t>Factor de ajuste</t>
-  </si>
-  <si>
-    <t>Horas total analista x día</t>
-  </si>
-  <si>
-    <t>Esfuerzo más probable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total de dia de dias pesimistas </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 personas se gastan </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Días </t>
+    <r>
+      <t>Actividades</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Frecuencia </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Esfuerzo Unidad </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Esfuerzo total</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Visión</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Reunión de entendimiento</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Plan de pruebas general</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <t> </t>
+  </si>
+  <si>
+    <r>
+      <t>Logística</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Asignación de rol analistas</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Ceremonias SCRUM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>7</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>1,5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Planteamiento Herramienta de pruebas</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Verificación de datos</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Preparaciones ambientes</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Planeación</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Cronograma de actividades</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Plan detallado de pruebas</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Reunión aprobación</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Diseño</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Pruebas funcionales - Riesgos</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>6</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Pruebas de Usabilidad - Riesgos</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Pruebas de Rendimiento - Riesgos</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Ejecución</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Pruebas exploratorias</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <t>smoke test</t>
+  </si>
+  <si>
+    <r>
+      <t>Pruebas Casos de uso</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Transición de Estados</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Usabilidad</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Pruebas de Rendimiento</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <t>Gestión</t>
+  </si>
+  <si>
+    <r>
+      <t>Reporte de issues</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Gestión de issues</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Entrega de prueba</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Informe resultados pruebas</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Esfuerzo estimado</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Factor de ajuste</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Horas total analista x día</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Esfuerzo más probable</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Total de dia de dias pesimistas </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>3 personas se gastan </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Días </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>4,7</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
   </si>
   <si>
     <t>1. Identificar</t>
@@ -836,9 +1385,6 @@
     <t>se deben mostrar los cursos que pertenezcan a esa categoría de ruta de aprendizaje.</t>
   </si>
   <si>
-    <t>REVISION DE ESPECIFICACIONES DE LA APP</t>
-  </si>
-  <si>
     <t>NRO</t>
   </si>
   <si>
@@ -878,7 +1424,7 @@
     <t>Daniel Sandoval</t>
   </si>
   <si>
-    <t>error</t>
+    <t>Falla</t>
   </si>
   <si>
     <t>Construcción</t>
@@ -900,7 +1446,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -967,18 +1513,6 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
       <charset val="1"/>
     </font>
     <font>
@@ -1019,6 +1553,22 @@
       <color rgb="FFFFFFFF"/>
       <name val="Arial Black"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="15">
     <fill>
@@ -1048,12 +1598,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1105,6 +1649,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD0CECE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="32">
     <border>
@@ -1459,7 +2009,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="135">
+  <cellXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1473,279 +2023,49 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1781,16 +2101,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1815,22 +2135,73 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1838,6 +2209,159 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="10" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="10" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="19" fillId="14" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="10" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4685,14 +5209,14 @@
   </cols>
   <sheetData>
     <row r="3" spans="4:10" ht="15.75">
-      <c r="D3" s="52" t="s">
+      <c r="D3" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
-      <c r="G3" s="52"/>
-      <c r="H3" s="52"/>
-      <c r="I3" s="52"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
       <c r="J3" s="4"/>
     </row>
     <row r="4" spans="4:10" ht="15.75">
@@ -5065,33 +5589,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:J8"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4:G8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="4" max="4" width="25.140625" customWidth="1"/>
     <col min="5" max="5" width="29.7109375" customWidth="1"/>
-    <col min="6" max="6" width="21.140625" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" customWidth="1"/>
     <col min="7" max="7" width="41.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:10">
-      <c r="C1" s="55" t="s">
+      <c r="C1" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
     </row>
     <row r="2" spans="2:10" ht="7.5" customHeight="1">
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
     </row>
     <row r="3" spans="2:10" ht="21.75" customHeight="1">
       <c r="B3" s="1"/>
@@ -5114,49 +5638,49 @@
       <c r="J3" s="1"/>
     </row>
     <row r="4" spans="2:10" ht="186" customHeight="1">
-      <c r="C4" s="53" t="s">
+      <c r="C4" s="50" t="s">
         <v>46</v>
       </c>
-      <c r="D4" s="58" t="s">
+      <c r="D4" s="55" t="s">
         <v>47</v>
       </c>
-      <c r="E4" s="56" t="s">
+      <c r="E4" s="53" t="s">
         <v>48</v>
       </c>
-      <c r="F4" s="56" t="s">
+      <c r="F4" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="G4" s="54" t="s">
+      <c r="G4" s="51" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="5" spans="2:10">
-      <c r="C5" s="53"/>
-      <c r="D5" s="59"/>
-      <c r="E5" s="57"/>
-      <c r="F5" s="57"/>
-      <c r="G5" s="54"/>
+      <c r="C5" s="50"/>
+      <c r="D5" s="56"/>
+      <c r="E5" s="54"/>
+      <c r="F5" s="54"/>
+      <c r="G5" s="51"/>
     </row>
     <row r="6" spans="2:10">
-      <c r="C6" s="53"/>
-      <c r="D6" s="59"/>
-      <c r="E6" s="57"/>
-      <c r="F6" s="57"/>
-      <c r="G6" s="54"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="56"/>
+      <c r="E6" s="54"/>
+      <c r="F6" s="54"/>
+      <c r="G6" s="51"/>
     </row>
     <row r="7" spans="2:10">
-      <c r="C7" s="53"/>
-      <c r="D7" s="59"/>
-      <c r="E7" s="57"/>
-      <c r="F7" s="57"/>
-      <c r="G7" s="54"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="56"/>
+      <c r="E7" s="54"/>
+      <c r="F7" s="54"/>
+      <c r="G7" s="51"/>
     </row>
     <row r="8" spans="2:10" ht="201.75" customHeight="1">
-      <c r="C8" s="53"/>
-      <c r="D8" s="59"/>
-      <c r="E8" s="57"/>
-      <c r="F8" s="57"/>
-      <c r="G8" s="54"/>
+      <c r="C8" s="50"/>
+      <c r="D8" s="56"/>
+      <c r="E8" s="54"/>
+      <c r="F8" s="54"/>
+      <c r="G8" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -5173,17 +5697,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CF52698-2E0D-4FCD-8927-B03F413D1A02}">
-  <dimension ref="D1:K38"/>
+  <dimension ref="D1:K39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="1.7109375" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" customWidth="1"/>
-    <col min="5" max="5" width="29.28515625" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" customWidth="1"/>
+    <col min="5" max="5" width="28" customWidth="1"/>
     <col min="6" max="6" width="12.5703125" customWidth="1"/>
     <col min="7" max="7" width="16" customWidth="1"/>
     <col min="8" max="8" width="14.85546875" customWidth="1"/>
@@ -5192,506 +5716,594 @@
     <row r="1" spans="4:11" ht="6.75" customHeight="1"/>
     <row r="2" spans="4:11" ht="0.75" customHeight="1"/>
     <row r="3" spans="4:11">
-      <c r="D3" s="62" t="s">
+      <c r="D3" s="98" t="s">
         <v>51</v>
       </c>
-      <c r="E3" s="63"/>
-      <c r="F3" s="46" t="s">
+      <c r="E3" s="99"/>
+      <c r="F3" s="85" t="s">
         <v>52</v>
       </c>
-      <c r="G3" s="47" t="s">
+      <c r="G3" s="85" t="s">
         <v>53</v>
       </c>
-      <c r="H3" s="48" t="s">
+      <c r="H3" s="85" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="4" spans="4:11" ht="13.5" customHeight="1">
-      <c r="D4" s="60" t="s">
+      <c r="D4" s="102" t="s">
         <v>55</v>
       </c>
-      <c r="E4" s="30" t="s">
+      <c r="E4" s="86" t="s">
         <v>56</v>
       </c>
-      <c r="F4" s="13">
+      <c r="F4" s="119" t="s">
+        <v>57</v>
+      </c>
+      <c r="G4" s="119" t="s">
+        <v>58</v>
+      </c>
+      <c r="H4" s="113">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="4:11" ht="16.5" customHeight="1">
+      <c r="D5" s="103"/>
+      <c r="E5" s="86" t="s">
+        <v>59</v>
+      </c>
+      <c r="F5" s="120" t="s">
+        <v>60</v>
+      </c>
+      <c r="G5" s="121" t="s">
+        <v>61</v>
+      </c>
+      <c r="H5" s="114">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="4:11">
+      <c r="D6" s="88" t="s">
+        <v>62</v>
+      </c>
+      <c r="E6" s="89" t="s">
+        <v>62</v>
+      </c>
+      <c r="F6" s="122" t="s">
+        <v>62</v>
+      </c>
+      <c r="G6" s="122" t="s">
+        <v>62</v>
+      </c>
+      <c r="H6" s="115" t="s">
+        <v>62</v>
+      </c>
+      <c r="K6" s="7"/>
+    </row>
+    <row r="7" spans="4:11" ht="16.5" customHeight="1">
+      <c r="D7" s="100" t="s">
+        <v>63</v>
+      </c>
+      <c r="E7" s="86" t="s">
+        <v>64</v>
+      </c>
+      <c r="F7" s="120" t="s">
+        <v>60</v>
+      </c>
+      <c r="G7" s="120" t="s">
+        <v>58</v>
+      </c>
+      <c r="H7" s="114">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="4:11" ht="17.25" customHeight="1">
+      <c r="D8" s="100"/>
+      <c r="E8" s="86" t="s">
+        <v>65</v>
+      </c>
+      <c r="F8" s="120" t="s">
+        <v>66</v>
+      </c>
+      <c r="G8" s="120" t="s">
+        <v>67</v>
+      </c>
+      <c r="H8" s="114">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="9" spans="4:11" ht="27" customHeight="1">
+      <c r="D9" s="100"/>
+      <c r="E9" s="86" t="s">
+        <v>68</v>
+      </c>
+      <c r="F9" s="120" t="s">
+        <v>60</v>
+      </c>
+      <c r="G9" s="120" t="s">
+        <v>58</v>
+      </c>
+      <c r="H9" s="114">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="4:11" ht="19.5" customHeight="1">
+      <c r="D10" s="100"/>
+      <c r="E10" s="86" t="s">
+        <v>69</v>
+      </c>
+      <c r="F10" s="120" t="s">
+        <v>60</v>
+      </c>
+      <c r="G10" s="120" t="s">
+        <v>57</v>
+      </c>
+      <c r="H10" s="114">
         <v>2</v>
       </c>
-      <c r="G4" s="13">
+    </row>
+    <row r="11" spans="4:11" ht="14.25" customHeight="1">
+      <c r="D11" s="100"/>
+      <c r="E11" s="86" t="s">
+        <v>70</v>
+      </c>
+      <c r="F11" s="120" t="s">
+        <v>60</v>
+      </c>
+      <c r="G11" s="120" t="s">
+        <v>58</v>
+      </c>
+      <c r="H11" s="114">
         <v>3</v>
       </c>
-      <c r="H4" s="8">
-        <f>(F4*G4)</f>
+    </row>
+    <row r="12" spans="4:11">
+      <c r="D12" s="101" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" s="89" t="s">
+        <v>62</v>
+      </c>
+      <c r="F12" s="122" t="s">
+        <v>62</v>
+      </c>
+      <c r="G12" s="122" t="s">
+        <v>62</v>
+      </c>
+      <c r="H12" s="115" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="4:11">
+      <c r="D13" s="100" t="s">
+        <v>71</v>
+      </c>
+      <c r="E13" s="86" t="s">
+        <v>72</v>
+      </c>
+      <c r="F13" s="120" t="s">
+        <v>60</v>
+      </c>
+      <c r="G13" s="120" t="s">
+        <v>58</v>
+      </c>
+      <c r="H13" s="114">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="4:11" ht="28.5" customHeight="1">
+      <c r="D14" s="100"/>
+      <c r="E14" s="86" t="s">
+        <v>73</v>
+      </c>
+      <c r="F14" s="120" t="s">
+        <v>60</v>
+      </c>
+      <c r="G14" s="120" t="s">
+        <v>61</v>
+      </c>
+      <c r="H14" s="114">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="4:11" ht="11.25" customHeight="1">
+      <c r="D15" s="100"/>
+      <c r="E15" s="86" t="s">
+        <v>74</v>
+      </c>
+      <c r="F15" s="120" t="s">
+        <v>60</v>
+      </c>
+      <c r="G15" s="120" t="s">
+        <v>57</v>
+      </c>
+      <c r="H15" s="114">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="4:11">
+      <c r="D16" s="88" t="s">
+        <v>62</v>
+      </c>
+      <c r="E16" s="89" t="s">
+        <v>62</v>
+      </c>
+      <c r="F16" s="122" t="s">
+        <v>62</v>
+      </c>
+      <c r="G16" s="122" t="s">
+        <v>62</v>
+      </c>
+      <c r="H16" s="115" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="4:8" ht="15" customHeight="1">
+      <c r="D17" s="100" t="s">
+        <v>75</v>
+      </c>
+      <c r="E17" s="86" t="s">
+        <v>76</v>
+      </c>
+      <c r="F17" s="120" t="s">
+        <v>77</v>
+      </c>
+      <c r="G17" s="120" t="s">
+        <v>78</v>
+      </c>
+      <c r="H17" s="114">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="4:8" ht="27" customHeight="1">
+      <c r="D18" s="100"/>
+      <c r="E18" s="87" t="s">
+        <v>79</v>
+      </c>
+      <c r="F18" s="120" t="s">
+        <v>57</v>
+      </c>
+      <c r="G18" s="120" t="s">
+        <v>58</v>
+      </c>
+      <c r="H18" s="114">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="4:11" ht="16.5" customHeight="1">
-      <c r="D5" s="61"/>
-      <c r="E5" s="30" t="s">
+    <row r="19" spans="4:8" ht="27.75" customHeight="1">
+      <c r="D19" s="100"/>
+      <c r="E19" s="86" t="s">
+        <v>80</v>
+      </c>
+      <c r="F19" s="120" t="s">
+        <v>58</v>
+      </c>
+      <c r="G19" s="120" t="s">
+        <v>61</v>
+      </c>
+      <c r="H19" s="114">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="4:8">
+      <c r="D20" s="88" t="s">
+        <v>62</v>
+      </c>
+      <c r="E20" s="89" t="s">
+        <v>62</v>
+      </c>
+      <c r="F20" s="122" t="s">
+        <v>62</v>
+      </c>
+      <c r="G20" s="122" t="s">
+        <v>62</v>
+      </c>
+      <c r="H20" s="115" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="4:8" ht="13.5" customHeight="1">
+      <c r="D21" s="118" t="s">
+        <v>81</v>
+      </c>
+      <c r="E21" s="86" t="s">
+        <v>82</v>
+      </c>
+      <c r="F21" s="120" t="s">
         <v>57</v>
       </c>
-      <c r="F5" s="13">
-        <v>1</v>
-      </c>
-      <c r="G5" s="32">
+      <c r="G21" s="120" t="s">
+        <v>58</v>
+      </c>
+      <c r="H21" s="114">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="4:8" ht="13.5" customHeight="1">
+      <c r="D22" s="118"/>
+      <c r="E22" s="86" t="s">
+        <v>83</v>
+      </c>
+      <c r="F22" s="120">
+        <v>2</v>
+      </c>
+      <c r="G22" s="120">
+        <v>3</v>
+      </c>
+      <c r="H22" s="114">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="4:8">
+      <c r="D23" s="118"/>
+      <c r="E23" s="87" t="s">
+        <v>84</v>
+      </c>
+      <c r="F23" s="120" t="s">
+        <v>58</v>
+      </c>
+      <c r="G23" s="120" t="s">
+        <v>78</v>
+      </c>
+      <c r="H23" s="114">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="4:8">
+      <c r="D24" s="118"/>
+      <c r="E24" s="86" t="s">
+        <v>85</v>
+      </c>
+      <c r="F24" s="120" t="s">
+        <v>57</v>
+      </c>
+      <c r="G24" s="120" t="s">
+        <v>58</v>
+      </c>
+      <c r="H24" s="114">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="4:8">
+      <c r="D25" s="118"/>
+      <c r="E25" s="86" t="s">
+        <v>86</v>
+      </c>
+      <c r="F25" s="120" t="s">
+        <v>57</v>
+      </c>
+      <c r="G25" s="120" t="s">
+        <v>58</v>
+      </c>
+      <c r="H25" s="114">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="4:8" ht="15.75" customHeight="1">
+      <c r="D26" s="118"/>
+      <c r="E26" s="87" t="s">
+        <v>87</v>
+      </c>
+      <c r="F26" s="120" t="s">
+        <v>57</v>
+      </c>
+      <c r="G26" s="120" t="s">
+        <v>61</v>
+      </c>
+      <c r="H26" s="114">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="4:8" ht="15.75" customHeight="1">
+      <c r="D27" s="88" t="s">
+        <v>62</v>
+      </c>
+      <c r="E27" s="89" t="s">
+        <v>62</v>
+      </c>
+      <c r="F27" s="122" t="s">
+        <v>62</v>
+      </c>
+      <c r="G27" s="122" t="s">
+        <v>62</v>
+      </c>
+      <c r="H27" s="115" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="4:8" ht="15.75" customHeight="1">
+      <c r="D28" s="105" t="s">
+        <v>88</v>
+      </c>
+      <c r="E28" s="86" t="s">
+        <v>89</v>
+      </c>
+      <c r="F28" s="120" t="s">
+        <v>57</v>
+      </c>
+      <c r="G28" s="120" t="s">
+        <v>57</v>
+      </c>
+      <c r="H28" s="114">
         <v>4</v>
       </c>
-      <c r="H5" s="8">
-        <f>(F5*G5)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="4:11">
-      <c r="D6" s="29"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="28"/>
-      <c r="K6" s="31"/>
-    </row>
-    <row r="7" spans="4:11" ht="16.5" customHeight="1">
-      <c r="D7" s="65" t="s">
-        <v>58</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="F7" s="14">
-        <v>1</v>
-      </c>
-      <c r="G7" s="14">
-        <v>3</v>
-      </c>
-      <c r="H7" s="8">
-        <f>F7*G7</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="4:11" ht="17.25" customHeight="1">
-      <c r="D8" s="65"/>
-      <c r="E8" s="13" t="s">
+    </row>
+    <row r="29" spans="4:8" ht="15.75" customHeight="1">
+      <c r="D29" s="105"/>
+      <c r="E29" s="86" t="s">
+        <v>90</v>
+      </c>
+      <c r="F29" s="120" t="s">
+        <v>57</v>
+      </c>
+      <c r="G29" s="120" t="s">
+        <v>61</v>
+      </c>
+      <c r="H29" s="114">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="4:8">
+      <c r="D30" s="88" t="s">
+        <v>62</v>
+      </c>
+      <c r="E30" s="89" t="s">
+        <v>62</v>
+      </c>
+      <c r="F30" s="122" t="s">
+        <v>62</v>
+      </c>
+      <c r="G30" s="122" t="s">
+        <v>62</v>
+      </c>
+      <c r="H30" s="115" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31" spans="4:8">
+      <c r="D31" s="91" t="s">
+        <v>91</v>
+      </c>
+      <c r="E31" s="86" t="s">
+        <v>92</v>
+      </c>
+      <c r="F31" s="120" t="s">
         <v>60</v>
       </c>
-      <c r="F8" s="14">
-        <v>7</v>
-      </c>
-      <c r="G8" s="14">
-        <v>1.5</v>
-      </c>
-      <c r="H8" s="8">
-        <f>F8*G8</f>
-        <v>10.5</v>
-      </c>
-    </row>
-    <row r="9" spans="4:11" ht="27" customHeight="1">
-      <c r="D9" s="65"/>
-      <c r="E9" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="F9" s="14">
-        <v>1</v>
-      </c>
-      <c r="G9" s="14">
-        <v>3</v>
-      </c>
-      <c r="H9" s="8">
-        <f>F9*G9</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="4:11" ht="19.5" customHeight="1">
-      <c r="D10" s="65"/>
-      <c r="E10" s="13" t="s">
+      <c r="G31" s="120" t="s">
+        <v>57</v>
+      </c>
+      <c r="H31" s="114">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="4:8">
+      <c r="D32" s="88" t="s">
         <v>62</v>
       </c>
-      <c r="F10" s="14">
-        <v>1</v>
-      </c>
-      <c r="G10" s="14">
-        <v>2</v>
-      </c>
-      <c r="H10" s="8">
-        <f>F10*G10</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="4:11" ht="14.25" customHeight="1">
-      <c r="D11" s="65"/>
-      <c r="E11" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="F11" s="14">
-        <v>1</v>
-      </c>
-      <c r="G11" s="14">
-        <v>3</v>
-      </c>
-      <c r="H11" s="8">
-        <f>F11*G11</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="4:11">
-      <c r="D12" s="25"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="28"/>
-    </row>
-    <row r="13" spans="4:11">
-      <c r="D13" s="65" t="s">
-        <v>64</v>
-      </c>
-      <c r="E13" s="37" t="s">
-        <v>65</v>
-      </c>
-      <c r="F13" s="13">
-        <v>1</v>
-      </c>
-      <c r="G13" s="14">
-        <v>3</v>
-      </c>
-      <c r="H13" s="8">
-        <f>G13*F13</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="4:11" ht="28.5" customHeight="1">
-      <c r="D14" s="65"/>
-      <c r="E14" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="F14" s="13">
-        <v>1</v>
-      </c>
-      <c r="G14" s="14">
-        <v>4</v>
-      </c>
-      <c r="H14" s="8">
-        <f>G14*F14</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="4:11" ht="11.25" customHeight="1">
-      <c r="D15" s="65"/>
-      <c r="E15" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="F15" s="13">
-        <v>1</v>
-      </c>
-      <c r="G15" s="14">
-        <v>2</v>
-      </c>
-      <c r="H15" s="8">
-        <f>G15*F15</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="4:11">
-      <c r="D16" s="25"/>
-      <c r="E16" s="41"/>
-      <c r="F16" s="42"/>
-      <c r="G16" s="42"/>
-      <c r="H16" s="43"/>
-    </row>
-    <row r="17" spans="4:8" ht="13.5" customHeight="1">
-      <c r="D17" s="61" t="s">
-        <v>68</v>
-      </c>
-      <c r="E17" s="30" t="s">
-        <v>69</v>
-      </c>
-      <c r="F17" s="15">
-        <v>6</v>
-      </c>
-      <c r="G17" s="15">
-        <v>5</v>
-      </c>
-      <c r="H17" s="16">
-        <f>F17*G17</f>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="4:8" ht="21" customHeight="1">
-      <c r="D18" s="61"/>
-      <c r="E18" s="38" t="s">
-        <v>70</v>
-      </c>
-      <c r="F18" s="14">
-        <v>2</v>
-      </c>
-      <c r="G18" s="15">
-        <v>3</v>
-      </c>
-      <c r="H18" s="16">
-        <f>F18*G18</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="4:8" ht="27.75" customHeight="1">
-      <c r="D19" s="61"/>
-      <c r="E19" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="F19" s="14">
-        <v>3</v>
-      </c>
-      <c r="G19" s="15">
-        <v>4</v>
-      </c>
-      <c r="H19" s="16">
-        <f>F19*G19</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="4:8">
-      <c r="D20" s="25"/>
-      <c r="E20" s="36"/>
-      <c r="F20" s="34"/>
-      <c r="G20" s="34"/>
-      <c r="H20" s="28"/>
-    </row>
-    <row r="21" spans="4:8" ht="13.5" customHeight="1">
-      <c r="D21" s="64" t="s">
-        <v>72</v>
-      </c>
-      <c r="E21" s="30" t="s">
-        <v>73</v>
-      </c>
-      <c r="F21" s="14">
-        <v>2</v>
-      </c>
-      <c r="G21" s="14">
-        <v>3</v>
-      </c>
-      <c r="H21" s="8">
-        <f>F21*G21</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="4:8">
-      <c r="D22" s="64"/>
-      <c r="E22" s="38" t="s">
-        <v>74</v>
-      </c>
-      <c r="F22" s="14">
-        <v>3</v>
-      </c>
-      <c r="G22" s="15">
-        <v>5</v>
-      </c>
-      <c r="H22" s="8">
-        <f>F22*G22</f>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" spans="4:8">
-      <c r="D23" s="64"/>
-      <c r="E23" s="37" t="s">
-        <v>75</v>
-      </c>
-      <c r="F23" s="14">
-        <v>2</v>
-      </c>
-      <c r="G23" s="15">
-        <v>3</v>
-      </c>
-      <c r="H23" s="8">
-        <f>F23*G23</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="4:8">
-      <c r="D24" s="64"/>
-      <c r="E24" s="39" t="s">
-        <v>76</v>
-      </c>
-      <c r="F24" s="14">
-        <v>2</v>
-      </c>
-      <c r="G24" s="15">
-        <v>3</v>
-      </c>
-      <c r="H24" s="8">
-        <f>F24*G24</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="4:8" ht="15.75" customHeight="1">
-      <c r="D25" s="64"/>
-      <c r="E25" s="38" t="s">
-        <v>77</v>
-      </c>
-      <c r="F25" s="14">
-        <v>2</v>
-      </c>
-      <c r="G25" s="15">
-        <v>4</v>
-      </c>
-      <c r="H25" s="8">
-        <f>F25*G25</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="4:8" ht="15.75" customHeight="1">
-      <c r="D26" s="25"/>
-      <c r="E26" s="36"/>
-      <c r="F26" s="34"/>
-      <c r="G26" s="34"/>
-      <c r="H26" s="28"/>
-    </row>
-    <row r="27" spans="4:8" ht="15.75" customHeight="1">
-      <c r="D27" s="33"/>
-      <c r="E27" s="40" t="s">
-        <v>78</v>
-      </c>
-      <c r="F27" s="35">
-        <v>2</v>
-      </c>
-      <c r="G27" s="35">
-        <v>2</v>
-      </c>
-      <c r="H27" s="8">
-        <f>F27*G27</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="4:8" ht="15.75" customHeight="1">
-      <c r="D28" s="33" t="s">
-        <v>79</v>
-      </c>
-      <c r="E28" s="40" t="s">
-        <v>80</v>
-      </c>
-      <c r="F28" s="35">
-        <v>2</v>
-      </c>
-      <c r="G28" s="35">
-        <v>4</v>
-      </c>
-      <c r="H28" s="8">
-        <f>F28*G28</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="29" spans="4:8">
-      <c r="D29" s="25"/>
-      <c r="E29" s="36"/>
-      <c r="F29" s="34"/>
-      <c r="G29" s="34"/>
-      <c r="H29" s="28"/>
-    </row>
-    <row r="30" spans="4:8">
-      <c r="D30" s="23" t="s">
-        <v>81</v>
-      </c>
-      <c r="E30" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="F30" s="14">
-        <v>1</v>
-      </c>
-      <c r="G30" s="14">
-        <v>2</v>
-      </c>
-      <c r="H30" s="8">
-        <f>F30*G30</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="4:8">
-      <c r="D31" s="44"/>
-      <c r="E31" s="27"/>
-      <c r="F31" s="27"/>
-      <c r="G31" s="26"/>
-      <c r="H31" s="28"/>
-    </row>
-    <row r="32" spans="4:8">
-      <c r="D32" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="12"/>
-      <c r="H32" s="17">
+      <c r="E32" s="89" t="s">
+        <v>62</v>
+      </c>
+      <c r="F32" s="89" t="s">
+        <v>62</v>
+      </c>
+      <c r="G32" s="89" t="s">
+        <v>62</v>
+      </c>
+      <c r="H32" s="90" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="33" spans="4:8">
+      <c r="D33" s="104" t="s">
+        <v>93</v>
+      </c>
+      <c r="E33" s="110"/>
+      <c r="F33" s="110"/>
+      <c r="G33" s="110"/>
+      <c r="H33" s="112">
         <f>SUM(H4:H31)</f>
-        <v>143.5</v>
-      </c>
-    </row>
-    <row r="33" spans="4:8">
-      <c r="D33" s="24" t="s">
-        <v>84</v>
-      </c>
-      <c r="E33" s="10"/>
-      <c r="F33" s="10"/>
-      <c r="G33" s="9"/>
-      <c r="H33" s="18">
-        <v>0.3</v>
+        <v>149.5</v>
       </c>
     </row>
     <row r="34" spans="4:8">
-      <c r="D34" s="45" t="s">
-        <v>85</v>
-      </c>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
-      <c r="G34" s="12"/>
-      <c r="H34" s="17">
-        <f>(3*9)</f>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="35" spans="4:8">
-      <c r="D35" s="44"/>
-      <c r="E35" s="27"/>
-      <c r="F35" s="27"/>
-      <c r="G35" s="26"/>
-      <c r="H35" s="28"/>
+      <c r="D34" s="100" t="s">
+        <v>94</v>
+      </c>
+      <c r="E34" s="109"/>
+      <c r="F34" s="109"/>
+      <c r="G34" s="109"/>
+      <c r="H34" s="117">
+        <f>RIESGOS!J12</f>
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="35" spans="4:8" ht="30.75" customHeight="1">
+      <c r="D35" s="107" t="s">
+        <v>95</v>
+      </c>
+      <c r="E35" s="108"/>
+      <c r="F35" s="108"/>
+      <c r="G35" s="108"/>
+      <c r="H35" s="112">
+        <f>(RIESGOS!K12)</f>
+        <v>28.404999999999998</v>
+      </c>
     </row>
     <row r="36" spans="4:8">
-      <c r="D36" s="45" t="s">
-        <v>86</v>
-      </c>
-      <c r="E36" s="7"/>
-      <c r="F36" s="7"/>
-      <c r="G36" s="12"/>
-      <c r="H36" s="17">
-        <f>H34+H32</f>
-        <v>170.5</v>
-      </c>
-    </row>
-    <row r="37" spans="4:8">
-      <c r="D37" s="66" t="s">
-        <v>87</v>
-      </c>
-      <c r="E37" s="67"/>
-      <c r="F37" s="10"/>
-      <c r="G37" s="9"/>
-      <c r="H37" s="11"/>
-    </row>
-    <row r="38" spans="4:8">
-      <c r="D38" s="19"/>
-      <c r="E38" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="F38" s="21"/>
-      <c r="G38" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="H38" s="22">
-        <f>H36/36</f>
-        <v>4.7361111111111107</v>
+      <c r="D36" s="88" t="s">
+        <v>62</v>
+      </c>
+      <c r="E36" s="89" t="s">
+        <v>62</v>
+      </c>
+      <c r="F36" s="89" t="s">
+        <v>62</v>
+      </c>
+      <c r="G36" s="89" t="s">
+        <v>62</v>
+      </c>
+      <c r="H36" s="90" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="37" spans="4:8" ht="30.75" customHeight="1">
+      <c r="D37" s="107" t="s">
+        <v>96</v>
+      </c>
+      <c r="E37" s="108"/>
+      <c r="F37" s="108"/>
+      <c r="G37" s="108"/>
+      <c r="H37" s="112">
+        <f>(H33+H35)</f>
+        <v>177.905</v>
+      </c>
+    </row>
+    <row r="38" spans="4:8" ht="30.75" customHeight="1">
+      <c r="D38" s="103" t="s">
+        <v>97</v>
+      </c>
+      <c r="E38" s="106"/>
+      <c r="F38" s="92" t="s">
+        <v>62</v>
+      </c>
+      <c r="G38" s="92" t="s">
+        <v>62</v>
+      </c>
+      <c r="H38" s="93" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="39" spans="4:8">
+      <c r="D39" s="94" t="s">
+        <v>62</v>
+      </c>
+      <c r="E39" s="95" t="s">
+        <v>98</v>
+      </c>
+      <c r="F39" s="96" t="s">
+        <v>62</v>
+      </c>
+      <c r="G39" s="95" t="s">
+        <v>99</v>
+      </c>
+      <c r="H39" s="97" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="D37:E37"/>
+  <mergeCells count="11">
+    <mergeCell ref="D38:E38"/>
     <mergeCell ref="D13:D15"/>
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="D17:D19"/>
-    <mergeCell ref="D21:D25"/>
     <mergeCell ref="D7:D11"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="D37:G37"/>
+    <mergeCell ref="D35:G35"/>
+    <mergeCell ref="D34:G34"/>
+    <mergeCell ref="D33:G33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5699,10 +6311,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC971A1E-ED3D-4010-BA68-569469E882F2}">
-  <dimension ref="B2:I21"/>
+  <dimension ref="B2:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:C5"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5713,397 +6325,486 @@
     <col min="7" max="7" width="13.140625" customWidth="1"/>
     <col min="8" max="8" width="15.42578125" customWidth="1"/>
     <col min="9" max="9" width="37.7109375" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9">
-      <c r="B2" s="78" t="s">
-        <v>90</v>
-      </c>
-      <c r="C2" s="79"/>
-      <c r="D2" s="79"/>
-      <c r="E2" s="79"/>
-      <c r="F2" s="80" t="s">
-        <v>91</v>
-      </c>
-      <c r="G2" s="80"/>
-      <c r="H2" s="80"/>
-      <c r="I2" s="81" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="3" spans="2:9" ht="20.25" customHeight="1">
-      <c r="B3" s="82" t="s">
-        <v>93</v>
-      </c>
-      <c r="C3" s="83"/>
-      <c r="D3" s="83"/>
-      <c r="E3" s="83"/>
-      <c r="F3" s="83"/>
-      <c r="G3" s="83"/>
-      <c r="H3" s="83"/>
-      <c r="I3" s="72"/>
-    </row>
-    <row r="4" spans="2:9" ht="29.25" customHeight="1">
-      <c r="B4" s="84" t="s">
-        <v>94</v>
-      </c>
-      <c r="C4" s="84"/>
-      <c r="D4" s="84" t="s">
-        <v>95</v>
-      </c>
-      <c r="E4" s="84"/>
-      <c r="F4" s="85" t="s">
-        <v>96</v>
-      </c>
-      <c r="G4" s="85" t="s">
-        <v>97</v>
-      </c>
-      <c r="H4" s="85" t="s">
-        <v>98</v>
-      </c>
-      <c r="I4" s="85" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="5" spans="2:9" ht="39" customHeight="1">
-      <c r="B5" s="133" t="s">
-        <v>100</v>
-      </c>
-      <c r="C5" s="134"/>
-      <c r="D5" s="69" t="s">
+    <row r="2" spans="2:11">
+      <c r="B2" s="73" t="s">
         <v>101</v>
       </c>
-      <c r="E5" s="69"/>
-      <c r="F5" s="49">
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="75" t="s">
+        <v>102</v>
+      </c>
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="14" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" ht="20.25" customHeight="1">
+      <c r="B3" s="76" t="s">
+        <v>104</v>
+      </c>
+      <c r="C3" s="77"/>
+      <c r="D3" s="77"/>
+      <c r="E3" s="77"/>
+      <c r="F3" s="77"/>
+      <c r="G3" s="77"/>
+      <c r="H3" s="77"/>
+      <c r="I3" s="78"/>
+    </row>
+    <row r="4" spans="2:11" ht="29.25" customHeight="1">
+      <c r="B4" s="79" t="s">
+        <v>105</v>
+      </c>
+      <c r="C4" s="79"/>
+      <c r="D4" s="79" t="s">
+        <v>106</v>
+      </c>
+      <c r="E4" s="79"/>
+      <c r="F4" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="I4" s="15" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" ht="39" customHeight="1">
+      <c r="B5" s="68" t="s">
+        <v>111</v>
+      </c>
+      <c r="C5" s="69"/>
+      <c r="D5" s="70" t="s">
+        <v>112</v>
+      </c>
+      <c r="E5" s="70"/>
+      <c r="F5" s="8">
         <v>3</v>
       </c>
-      <c r="G5" s="49">
+      <c r="G5" s="8">
         <v>3</v>
       </c>
-      <c r="H5" s="50">
+      <c r="H5" s="9">
         <f>G5*F5</f>
         <v>9</v>
       </c>
-      <c r="I5" s="51" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="6" spans="2:9" ht="31.5" customHeight="1">
-      <c r="B6" s="68" t="s">
-        <v>103</v>
-      </c>
-      <c r="C6" s="69"/>
-      <c r="D6" s="71" t="s">
-        <v>104</v>
-      </c>
-      <c r="E6" s="71"/>
-      <c r="F6" s="49">
+      <c r="I5" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="J5" s="111">
+        <v>0.03</v>
+      </c>
+      <c r="K5" s="116">
+        <f>J5*ESTIMACION!$H$33</f>
+        <v>4.4849999999999994</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="31.5" customHeight="1">
+      <c r="B6" s="71" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6" s="70"/>
+      <c r="D6" s="72" t="s">
+        <v>115</v>
+      </c>
+      <c r="E6" s="72"/>
+      <c r="F6" s="8">
         <v>3</v>
       </c>
-      <c r="G6" s="49">
+      <c r="G6" s="8">
         <v>3</v>
       </c>
-      <c r="H6" s="50">
+      <c r="H6" s="9">
         <f>G6*F6</f>
         <v>9</v>
       </c>
-      <c r="I6" s="51" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9" ht="40.5" customHeight="1">
-      <c r="B7" s="68" t="s">
-        <v>106</v>
-      </c>
-      <c r="C7" s="69"/>
-      <c r="D7" s="69" t="s">
-        <v>107</v>
-      </c>
-      <c r="E7" s="69"/>
-      <c r="F7" s="49">
+      <c r="I6" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="J6" s="111">
+        <v>0.03</v>
+      </c>
+      <c r="K6" s="116">
+        <f>J6*ESTIMACION!$H$33</f>
+        <v>4.4849999999999994</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" ht="40.5" customHeight="1">
+      <c r="B7" s="71" t="s">
+        <v>117</v>
+      </c>
+      <c r="C7" s="70"/>
+      <c r="D7" s="70" t="s">
+        <v>118</v>
+      </c>
+      <c r="E7" s="70"/>
+      <c r="F7" s="8">
         <v>1</v>
       </c>
-      <c r="G7" s="49">
+      <c r="G7" s="8">
         <v>3</v>
       </c>
-      <c r="H7" s="50">
+      <c r="H7" s="9">
         <f>G7*F7</f>
         <v>3</v>
       </c>
-      <c r="I7" s="51" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9" ht="54.75" customHeight="1">
-      <c r="B8" s="68" t="s">
-        <v>109</v>
-      </c>
-      <c r="C8" s="69"/>
-      <c r="D8" s="69" t="s">
-        <v>110</v>
-      </c>
-      <c r="E8" s="69"/>
-      <c r="F8" s="49">
+      <c r="I7" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="J7" s="111">
+        <v>0.01</v>
+      </c>
+      <c r="K7" s="116">
+        <f>J7*ESTIMACION!$H$33</f>
+        <v>1.4950000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" ht="54.75" customHeight="1">
+      <c r="B8" s="71" t="s">
+        <v>120</v>
+      </c>
+      <c r="C8" s="70"/>
+      <c r="D8" s="70" t="s">
+        <v>121</v>
+      </c>
+      <c r="E8" s="70"/>
+      <c r="F8" s="8">
         <v>3</v>
       </c>
-      <c r="G8" s="49">
+      <c r="G8" s="8">
         <v>3</v>
       </c>
-      <c r="H8" s="50">
+      <c r="H8" s="9">
         <f>G8*F8</f>
         <v>9</v>
       </c>
-      <c r="I8" s="51" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9" ht="30" customHeight="1">
-      <c r="B9" s="70" t="s">
-        <v>112</v>
-      </c>
-      <c r="C9" s="71"/>
-      <c r="D9" s="71" t="s">
-        <v>113</v>
-      </c>
-      <c r="E9" s="71"/>
-      <c r="F9" s="49">
+      <c r="I8" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="J8" s="111">
+        <v>0.03</v>
+      </c>
+      <c r="K8" s="116">
+        <f>J8*ESTIMACION!$H$33</f>
+        <v>4.4849999999999994</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" ht="30" customHeight="1">
+      <c r="B9" s="82" t="s">
+        <v>123</v>
+      </c>
+      <c r="C9" s="72"/>
+      <c r="D9" s="72" t="s">
+        <v>124</v>
+      </c>
+      <c r="E9" s="72"/>
+      <c r="F9" s="8">
         <v>3</v>
       </c>
-      <c r="G9" s="49">
+      <c r="G9" s="8">
         <v>2</v>
       </c>
-      <c r="H9" s="50">
+      <c r="H9" s="9">
         <f>G9*F9</f>
         <v>6</v>
       </c>
-      <c r="I9" s="51" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="10" spans="2:9" ht="30.75" customHeight="1">
-      <c r="B10" s="70" t="s">
-        <v>115</v>
-      </c>
-      <c r="C10" s="71"/>
-      <c r="D10" s="71" t="s">
-        <v>116</v>
-      </c>
-      <c r="E10" s="71"/>
-      <c r="F10" s="49">
+      <c r="I9" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="J9" s="111">
+        <v>0.03</v>
+      </c>
+      <c r="K9" s="116">
+        <f>J9*ESTIMACION!$H$33</f>
+        <v>4.4849999999999994</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" ht="30.75" customHeight="1">
+      <c r="B10" s="82" t="s">
+        <v>126</v>
+      </c>
+      <c r="C10" s="72"/>
+      <c r="D10" s="72" t="s">
+        <v>127</v>
+      </c>
+      <c r="E10" s="72"/>
+      <c r="F10" s="8">
         <v>3</v>
       </c>
-      <c r="G10" s="49">
+      <c r="G10" s="8">
         <v>3</v>
       </c>
-      <c r="H10" s="50">
+      <c r="H10" s="9">
         <f>G10*F10</f>
         <v>9</v>
       </c>
-      <c r="I10" s="51" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9" ht="39.75" customHeight="1">
-      <c r="B11" s="73" t="s">
-        <v>118</v>
-      </c>
-      <c r="C11" s="74"/>
-      <c r="D11" s="74" t="s">
-        <v>119</v>
-      </c>
-      <c r="E11" s="74"/>
-      <c r="F11" s="75">
+      <c r="I10" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="J10" s="111">
+        <v>0.03</v>
+      </c>
+      <c r="K10" s="116">
+        <f>J10*ESTIMACION!$H$33</f>
+        <v>4.4849999999999994</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" ht="39.75" customHeight="1">
+      <c r="B11" s="80" t="s">
+        <v>129</v>
+      </c>
+      <c r="C11" s="81"/>
+      <c r="D11" s="81" t="s">
+        <v>130</v>
+      </c>
+      <c r="E11" s="81"/>
+      <c r="F11" s="11">
         <v>3</v>
       </c>
-      <c r="G11" s="75">
+      <c r="G11" s="11">
         <v>2</v>
       </c>
-      <c r="H11" s="76">
+      <c r="H11" s="12">
         <f>G11*F11</f>
         <v>6</v>
       </c>
-      <c r="I11" s="77" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="13" spans="2:9">
-      <c r="B13" s="86" t="s">
-        <v>121</v>
-      </c>
-      <c r="C13" s="87"/>
-      <c r="D13" s="87"/>
-      <c r="E13" s="87"/>
-      <c r="F13" s="87"/>
-      <c r="G13" s="87"/>
-      <c r="H13" s="87"/>
-      <c r="I13" s="88"/>
-    </row>
-    <row r="14" spans="2:9" ht="28.5">
-      <c r="B14" s="97" t="s">
-        <v>94</v>
-      </c>
-      <c r="C14" s="98"/>
-      <c r="D14" s="98" t="s">
-        <v>95</v>
-      </c>
-      <c r="E14" s="98"/>
-      <c r="F14" s="99" t="s">
-        <v>96</v>
-      </c>
-      <c r="G14" s="99" t="s">
-        <v>97</v>
-      </c>
-      <c r="H14" s="99" t="s">
-        <v>98</v>
-      </c>
-      <c r="I14" s="100" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="15" spans="2:9" ht="42" customHeight="1">
-      <c r="B15" s="91" t="s">
-        <v>122</v>
-      </c>
-      <c r="C15" s="89"/>
-      <c r="D15" s="89" t="s">
-        <v>123</v>
-      </c>
-      <c r="E15" s="89"/>
-      <c r="F15" s="101">
+      <c r="I11" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="J11" s="111">
+        <v>0.03</v>
+      </c>
+      <c r="K11" s="116">
+        <f>J11*ESTIMACION!$H$33</f>
+        <v>4.4849999999999994</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11">
+      <c r="J12" s="111">
+        <f>SUM(J5:J11)</f>
+        <v>0.19</v>
+      </c>
+      <c r="K12" s="116">
+        <f>SUM(K5:K11)</f>
+        <v>28.404999999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11">
+      <c r="B13" s="63" t="s">
+        <v>132</v>
+      </c>
+      <c r="C13" s="64"/>
+      <c r="D13" s="64"/>
+      <c r="E13" s="64"/>
+      <c r="F13" s="64"/>
+      <c r="G13" s="64"/>
+      <c r="H13" s="64"/>
+      <c r="I13" s="65"/>
+    </row>
+    <row r="14" spans="2:11" ht="28.5">
+      <c r="B14" s="66" t="s">
+        <v>105</v>
+      </c>
+      <c r="C14" s="67"/>
+      <c r="D14" s="67" t="s">
+        <v>106</v>
+      </c>
+      <c r="E14" s="67"/>
+      <c r="F14" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="G14" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="H14" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="I14" s="21" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" ht="42" customHeight="1">
+      <c r="B15" s="61" t="s">
+        <v>133</v>
+      </c>
+      <c r="C15" s="59"/>
+      <c r="D15" s="59" t="s">
+        <v>134</v>
+      </c>
+      <c r="E15" s="59"/>
+      <c r="F15" s="16">
         <v>2</v>
       </c>
-      <c r="G15" s="101">
+      <c r="G15" s="16">
         <v>3</v>
       </c>
-      <c r="H15" s="92">
+      <c r="H15" s="17">
         <f>G15*F15</f>
         <v>6</v>
       </c>
-      <c r="I15" s="104" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="16" spans="2:9" ht="42" customHeight="1">
-      <c r="B16" s="93" t="s">
-        <v>125</v>
-      </c>
-      <c r="C16" s="94"/>
-      <c r="D16" s="94" t="s">
-        <v>126</v>
-      </c>
-      <c r="E16" s="94"/>
-      <c r="F16" s="102">
+      <c r="I15" s="22" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" ht="42" customHeight="1">
+      <c r="B16" s="62" t="s">
+        <v>136</v>
+      </c>
+      <c r="C16" s="60"/>
+      <c r="D16" s="60" t="s">
+        <v>137</v>
+      </c>
+      <c r="E16" s="60"/>
+      <c r="F16" s="18">
         <v>3</v>
       </c>
-      <c r="G16" s="102">
+      <c r="G16" s="18">
         <v>3</v>
       </c>
-      <c r="H16" s="90">
+      <c r="H16" s="9">
         <f t="shared" ref="H16:H20" si="0">G16*F16</f>
         <v>9</v>
       </c>
-      <c r="I16" s="105" t="s">
-        <v>127</v>
+      <c r="I16" s="23" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="17" spans="2:9" ht="47.25" customHeight="1">
-      <c r="B17" s="93" t="s">
-        <v>128</v>
-      </c>
-      <c r="C17" s="94"/>
-      <c r="D17" s="94" t="s">
-        <v>129</v>
-      </c>
-      <c r="E17" s="94"/>
-      <c r="F17" s="102">
+      <c r="B17" s="62" t="s">
+        <v>139</v>
+      </c>
+      <c r="C17" s="60"/>
+      <c r="D17" s="60" t="s">
+        <v>140</v>
+      </c>
+      <c r="E17" s="60"/>
+      <c r="F17" s="18">
         <v>3</v>
       </c>
-      <c r="G17" s="102">
+      <c r="G17" s="18">
         <v>2</v>
       </c>
-      <c r="H17" s="90">
+      <c r="H17" s="9">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="I17" s="105" t="s">
-        <v>130</v>
+      <c r="I17" s="23" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="18" spans="2:9" ht="51" customHeight="1">
-      <c r="B18" s="93" t="s">
-        <v>131</v>
-      </c>
-      <c r="C18" s="94"/>
-      <c r="D18" s="94" t="s">
-        <v>132</v>
-      </c>
-      <c r="E18" s="94"/>
-      <c r="F18" s="102">
+      <c r="B18" s="62" t="s">
+        <v>142</v>
+      </c>
+      <c r="C18" s="60"/>
+      <c r="D18" s="60" t="s">
+        <v>143</v>
+      </c>
+      <c r="E18" s="60"/>
+      <c r="F18" s="18">
         <v>3</v>
       </c>
-      <c r="G18" s="102">
+      <c r="G18" s="18">
         <v>2</v>
       </c>
-      <c r="H18" s="90">
+      <c r="H18" s="9">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="I18" s="105" t="s">
-        <v>133</v>
+      <c r="I18" s="23" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="19" spans="2:9" ht="42.75" customHeight="1">
-      <c r="B19" s="93" t="s">
-        <v>134</v>
-      </c>
-      <c r="C19" s="94"/>
-      <c r="D19" s="94" t="s">
-        <v>135</v>
-      </c>
-      <c r="E19" s="94"/>
-      <c r="F19" s="102">
+      <c r="B19" s="62" t="s">
+        <v>145</v>
+      </c>
+      <c r="C19" s="60"/>
+      <c r="D19" s="60" t="s">
+        <v>146</v>
+      </c>
+      <c r="E19" s="60"/>
+      <c r="F19" s="18">
         <v>2</v>
       </c>
-      <c r="G19" s="102">
+      <c r="G19" s="18">
         <v>3</v>
       </c>
-      <c r="H19" s="90">
+      <c r="H19" s="9">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="I19" s="105" t="s">
-        <v>136</v>
+      <c r="I19" s="23" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="20" spans="2:9" ht="43.5" customHeight="1">
-      <c r="B20" s="95" t="s">
-        <v>137</v>
-      </c>
-      <c r="C20" s="96"/>
-      <c r="D20" s="96" t="s">
-        <v>138</v>
-      </c>
-      <c r="E20" s="96"/>
-      <c r="F20" s="103">
+      <c r="B20" s="57" t="s">
+        <v>148</v>
+      </c>
+      <c r="C20" s="58"/>
+      <c r="D20" s="58" t="s">
+        <v>149</v>
+      </c>
+      <c r="E20" s="58"/>
+      <c r="F20" s="19">
         <v>2</v>
       </c>
-      <c r="G20" s="103">
+      <c r="G20" s="19">
         <v>2</v>
       </c>
-      <c r="H20" s="76">
+      <c r="H20" s="12">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="I20" s="106" t="s">
-        <v>139</v>
+      <c r="I20" s="24" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="21" spans="2:9">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
     </row>
+    <row r="33" spans="8:8">
+      <c r="H33" s="111">
+        <f>(RIESGOS!J12)</f>
+        <v>0.19</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="B3:I3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="B13:I13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="D15:E15"/>
     <mergeCell ref="D16:E16"/>
@@ -6116,28 +6817,6 @@
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B13:I13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="B3:I3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D11:E11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6160,59 +6839,59 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5">
-      <c r="B2" s="115" t="s">
-        <v>140</v>
-      </c>
-      <c r="C2" s="116" t="s">
-        <v>141</v>
-      </c>
-      <c r="D2" s="116" t="s">
-        <v>142</v>
-      </c>
-      <c r="E2" s="117" t="s">
-        <v>143</v>
+      <c r="B2" s="33" t="s">
+        <v>151</v>
+      </c>
+      <c r="C2" s="34" t="s">
+        <v>152</v>
+      </c>
+      <c r="D2" s="34" t="s">
+        <v>153</v>
+      </c>
+      <c r="E2" s="35" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="3" spans="2:5" ht="72">
-      <c r="B3" s="109">
+      <c r="B3" s="27">
         <v>1</v>
       </c>
-      <c r="C3" s="107" t="s">
-        <v>144</v>
-      </c>
-      <c r="D3" s="108" t="s">
-        <v>145</v>
-      </c>
-      <c r="E3" s="110" t="s">
-        <v>146</v>
+      <c r="C3" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>156</v>
+      </c>
+      <c r="E3" s="28" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="4" spans="2:5" ht="115.5">
-      <c r="B4" s="109">
+      <c r="B4" s="27">
         <v>2</v>
       </c>
-      <c r="C4" s="107" t="s">
-        <v>147</v>
-      </c>
-      <c r="D4" s="108" t="s">
-        <v>148</v>
-      </c>
-      <c r="E4" s="110" t="s">
-        <v>149</v>
+      <c r="C4" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="D4" s="26" t="s">
+        <v>159</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="5" spans="2:5" ht="129.75">
-      <c r="B5" s="111">
+      <c r="B5" s="29">
         <v>3</v>
       </c>
-      <c r="C5" s="112" t="s">
-        <v>150</v>
-      </c>
-      <c r="D5" s="113" t="s">
-        <v>151</v>
-      </c>
-      <c r="E5" s="114" t="s">
-        <v>152</v>
+      <c r="C5" s="30" t="s">
+        <v>161</v>
+      </c>
+      <c r="D5" s="31" t="s">
+        <v>162</v>
+      </c>
+      <c r="E5" s="32" t="s">
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -6227,8 +6906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58D9BC44-7C49-4BD4-811C-DAECB2CEE96F}">
   <dimension ref="B2:O10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6251,297 +6930,297 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" ht="18.75" customHeight="1">
-      <c r="B2" s="118" t="s">
-        <v>153</v>
-      </c>
-      <c r="C2" s="119" t="s">
-        <v>154</v>
-      </c>
-      <c r="E2" s="118" t="s">
-        <v>153</v>
-      </c>
-      <c r="F2" s="119" t="s">
-        <v>155</v>
-      </c>
-      <c r="H2" s="118" t="s">
-        <v>153</v>
-      </c>
-      <c r="I2" s="119" t="s">
-        <v>156</v>
-      </c>
-      <c r="K2" s="118" t="s">
-        <v>153</v>
-      </c>
-      <c r="L2" s="119" t="s">
-        <v>157</v>
-      </c>
-      <c r="N2" s="118" t="s">
-        <v>153</v>
-      </c>
-      <c r="O2" s="119" t="s">
-        <v>158</v>
+      <c r="B2" s="36" t="s">
+        <v>164</v>
+      </c>
+      <c r="C2" s="37" t="s">
+        <v>165</v>
+      </c>
+      <c r="E2" s="36" t="s">
+        <v>164</v>
+      </c>
+      <c r="F2" s="37" t="s">
+        <v>166</v>
+      </c>
+      <c r="H2" s="36" t="s">
+        <v>164</v>
+      </c>
+      <c r="I2" s="37" t="s">
+        <v>167</v>
+      </c>
+      <c r="K2" s="36" t="s">
+        <v>164</v>
+      </c>
+      <c r="L2" s="37" t="s">
+        <v>168</v>
+      </c>
+      <c r="N2" s="36" t="s">
+        <v>164</v>
+      </c>
+      <c r="O2" s="37" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="3" spans="2:15" ht="30.75" customHeight="1">
-      <c r="B3" s="118" t="s">
-        <v>159</v>
-      </c>
-      <c r="C3" s="124" t="s">
-        <v>160</v>
-      </c>
-      <c r="E3" s="118" t="s">
-        <v>159</v>
-      </c>
-      <c r="F3" s="121" t="s">
-        <v>161</v>
-      </c>
-      <c r="H3" s="118" t="s">
-        <v>159</v>
-      </c>
-      <c r="I3" s="121" t="s">
-        <v>162</v>
-      </c>
-      <c r="K3" s="118" t="s">
-        <v>159</v>
-      </c>
-      <c r="L3" s="121" t="s">
-        <v>163</v>
-      </c>
-      <c r="N3" s="118" t="s">
-        <v>159</v>
-      </c>
-      <c r="O3" s="121" t="s">
-        <v>164</v>
+      <c r="B3" s="36" t="s">
+        <v>170</v>
+      </c>
+      <c r="C3" s="42" t="s">
+        <v>171</v>
+      </c>
+      <c r="E3" s="36" t="s">
+        <v>170</v>
+      </c>
+      <c r="F3" s="39" t="s">
+        <v>172</v>
+      </c>
+      <c r="H3" s="36" t="s">
+        <v>170</v>
+      </c>
+      <c r="I3" s="39" t="s">
+        <v>173</v>
+      </c>
+      <c r="K3" s="36" t="s">
+        <v>170</v>
+      </c>
+      <c r="L3" s="39" t="s">
+        <v>174</v>
+      </c>
+      <c r="N3" s="36" t="s">
+        <v>170</v>
+      </c>
+      <c r="O3" s="39" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="4" spans="2:15" ht="15.75" customHeight="1">
-      <c r="B4" s="118" t="s">
-        <v>165</v>
-      </c>
-      <c r="C4" s="124" t="s">
-        <v>166</v>
-      </c>
-      <c r="E4" s="118" t="s">
-        <v>165</v>
-      </c>
-      <c r="F4" s="120" t="s">
-        <v>166</v>
-      </c>
-      <c r="H4" s="118" t="s">
-        <v>165</v>
-      </c>
-      <c r="I4" s="120" t="s">
-        <v>166</v>
-      </c>
-      <c r="K4" s="118" t="s">
-        <v>165</v>
-      </c>
-      <c r="L4" s="120" t="s">
-        <v>167</v>
-      </c>
-      <c r="N4" s="118" t="s">
-        <v>165</v>
-      </c>
-      <c r="O4" s="120" t="s">
-        <v>166</v>
+      <c r="B4" s="36" t="s">
+        <v>176</v>
+      </c>
+      <c r="C4" s="42" t="s">
+        <v>177</v>
+      </c>
+      <c r="E4" s="36" t="s">
+        <v>176</v>
+      </c>
+      <c r="F4" s="38" t="s">
+        <v>177</v>
+      </c>
+      <c r="H4" s="36" t="s">
+        <v>176</v>
+      </c>
+      <c r="I4" s="38" t="s">
+        <v>177</v>
+      </c>
+      <c r="K4" s="36" t="s">
+        <v>176</v>
+      </c>
+      <c r="L4" s="38" t="s">
+        <v>178</v>
+      </c>
+      <c r="N4" s="36" t="s">
+        <v>176</v>
+      </c>
+      <c r="O4" s="38" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="5" spans="2:15" ht="20.25" customHeight="1">
-      <c r="B5" s="118" t="s">
-        <v>168</v>
-      </c>
-      <c r="C5" s="124" t="s">
-        <v>169</v>
-      </c>
-      <c r="E5" s="118" t="s">
-        <v>168</v>
-      </c>
-      <c r="F5" s="120" t="s">
-        <v>169</v>
-      </c>
-      <c r="H5" s="118" t="s">
-        <v>168</v>
-      </c>
-      <c r="I5" s="120" t="s">
-        <v>169</v>
-      </c>
-      <c r="K5" s="118" t="s">
-        <v>168</v>
-      </c>
-      <c r="L5" s="120" t="s">
-        <v>169</v>
-      </c>
-      <c r="N5" s="118" t="s">
-        <v>168</v>
-      </c>
-      <c r="O5" s="120" t="s">
-        <v>169</v>
+      <c r="B5" s="36" t="s">
+        <v>179</v>
+      </c>
+      <c r="C5" s="42" t="s">
+        <v>180</v>
+      </c>
+      <c r="E5" s="36" t="s">
+        <v>179</v>
+      </c>
+      <c r="F5" s="38" t="s">
+        <v>180</v>
+      </c>
+      <c r="H5" s="36" t="s">
+        <v>179</v>
+      </c>
+      <c r="I5" s="38" t="s">
+        <v>180</v>
+      </c>
+      <c r="K5" s="36" t="s">
+        <v>179</v>
+      </c>
+      <c r="L5" s="38" t="s">
+        <v>180</v>
+      </c>
+      <c r="N5" s="36" t="s">
+        <v>179</v>
+      </c>
+      <c r="O5" s="38" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="6" spans="2:15" ht="126" customHeight="1">
-      <c r="B6" s="118" t="s">
-        <v>170</v>
-      </c>
-      <c r="C6" s="122" t="s">
-        <v>171</v>
-      </c>
-      <c r="E6" s="118" t="s">
-        <v>170</v>
-      </c>
-      <c r="F6" s="126" t="s">
-        <v>171</v>
-      </c>
-      <c r="H6" s="118" t="s">
-        <v>170</v>
-      </c>
-      <c r="I6" s="126" t="s">
-        <v>171</v>
-      </c>
-      <c r="K6" s="118" t="s">
-        <v>170</v>
-      </c>
-      <c r="L6" s="126" t="s">
-        <v>171</v>
-      </c>
-      <c r="N6" s="118" t="s">
-        <v>170</v>
-      </c>
-      <c r="O6" s="126" t="s">
-        <v>172</v>
+      <c r="B6" s="36" t="s">
+        <v>181</v>
+      </c>
+      <c r="C6" s="40" t="s">
+        <v>182</v>
+      </c>
+      <c r="E6" s="36" t="s">
+        <v>181</v>
+      </c>
+      <c r="F6" s="44" t="s">
+        <v>182</v>
+      </c>
+      <c r="H6" s="36" t="s">
+        <v>181</v>
+      </c>
+      <c r="I6" s="44" t="s">
+        <v>182</v>
+      </c>
+      <c r="K6" s="36" t="s">
+        <v>181</v>
+      </c>
+      <c r="L6" s="44" t="s">
+        <v>182</v>
+      </c>
+      <c r="N6" s="36" t="s">
+        <v>181</v>
+      </c>
+      <c r="O6" s="44" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="7" spans="2:15" ht="36.75" customHeight="1">
-      <c r="B7" s="118" t="s">
-        <v>173</v>
-      </c>
-      <c r="C7" s="125" t="s">
-        <v>174</v>
-      </c>
-      <c r="E7" s="118" t="s">
-        <v>173</v>
-      </c>
-      <c r="F7" s="122" t="s">
-        <v>175</v>
-      </c>
-      <c r="H7" s="118" t="s">
-        <v>173</v>
-      </c>
-      <c r="I7" s="122" t="s">
-        <v>176</v>
-      </c>
-      <c r="K7" s="118" t="s">
-        <v>173</v>
-      </c>
-      <c r="L7" s="122" t="s">
-        <v>176</v>
-      </c>
-      <c r="N7" s="118" t="s">
-        <v>173</v>
-      </c>
-      <c r="O7" s="122" t="s">
-        <v>177</v>
+      <c r="B7" s="36" t="s">
+        <v>184</v>
+      </c>
+      <c r="C7" s="43" t="s">
+        <v>185</v>
+      </c>
+      <c r="E7" s="36" t="s">
+        <v>184</v>
+      </c>
+      <c r="F7" s="40" t="s">
+        <v>186</v>
+      </c>
+      <c r="H7" s="36" t="s">
+        <v>184</v>
+      </c>
+      <c r="I7" s="40" t="s">
+        <v>187</v>
+      </c>
+      <c r="K7" s="36" t="s">
+        <v>184</v>
+      </c>
+      <c r="L7" s="40" t="s">
+        <v>187</v>
+      </c>
+      <c r="N7" s="36" t="s">
+        <v>184</v>
+      </c>
+      <c r="O7" s="40" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="8" spans="2:15" ht="123" customHeight="1">
-      <c r="B8" s="118" t="s">
-        <v>178</v>
-      </c>
-      <c r="C8" s="125" t="s">
-        <v>179</v>
-      </c>
-      <c r="E8" s="118" t="s">
-        <v>178</v>
-      </c>
-      <c r="F8" s="122" t="s">
-        <v>180</v>
-      </c>
-      <c r="H8" s="118" t="s">
-        <v>178</v>
-      </c>
-      <c r="I8" s="122" t="s">
-        <v>181</v>
-      </c>
-      <c r="K8" s="118" t="s">
-        <v>178</v>
-      </c>
-      <c r="L8" s="122" t="s">
-        <v>182</v>
-      </c>
-      <c r="N8" s="118" t="s">
-        <v>178</v>
-      </c>
-      <c r="O8" s="122" t="s">
-        <v>183</v>
+      <c r="B8" s="36" t="s">
+        <v>189</v>
+      </c>
+      <c r="C8" s="43" t="s">
+        <v>190</v>
+      </c>
+      <c r="E8" s="36" t="s">
+        <v>189</v>
+      </c>
+      <c r="F8" s="40" t="s">
+        <v>191</v>
+      </c>
+      <c r="H8" s="36" t="s">
+        <v>189</v>
+      </c>
+      <c r="I8" s="40" t="s">
+        <v>192</v>
+      </c>
+      <c r="K8" s="36" t="s">
+        <v>189</v>
+      </c>
+      <c r="L8" s="40" t="s">
+        <v>193</v>
+      </c>
+      <c r="N8" s="36" t="s">
+        <v>189</v>
+      </c>
+      <c r="O8" s="40" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="9" spans="2:15" ht="156" customHeight="1">
-      <c r="B9" s="118" t="s">
-        <v>184</v>
-      </c>
-      <c r="C9" s="125" t="s">
-        <v>185</v>
-      </c>
-      <c r="E9" s="118" t="s">
-        <v>184</v>
-      </c>
-      <c r="F9" s="125" t="s">
-        <v>186</v>
+      <c r="B9" s="36" t="s">
+        <v>195</v>
+      </c>
+      <c r="C9" s="43" t="s">
+        <v>196</v>
+      </c>
+      <c r="E9" s="36" t="s">
+        <v>195</v>
+      </c>
+      <c r="F9" s="43" t="s">
+        <v>197</v>
       </c>
       <c r="G9" s="1"/>
-      <c r="H9" s="118" t="s">
-        <v>184</v>
-      </c>
-      <c r="I9" s="125" t="s">
-        <v>187</v>
+      <c r="H9" s="36" t="s">
+        <v>195</v>
+      </c>
+      <c r="I9" s="43" t="s">
+        <v>198</v>
       </c>
       <c r="J9" s="1"/>
-      <c r="K9" s="118" t="s">
-        <v>184</v>
-      </c>
-      <c r="L9" s="125" t="s">
-        <v>188</v>
+      <c r="K9" s="36" t="s">
+        <v>195</v>
+      </c>
+      <c r="L9" s="43" t="s">
+        <v>199</v>
       </c>
       <c r="M9" s="1"/>
-      <c r="N9" s="118" t="s">
-        <v>184</v>
-      </c>
-      <c r="O9" s="125" t="s">
-        <v>189</v>
+      <c r="N9" s="36" t="s">
+        <v>195</v>
+      </c>
+      <c r="O9" s="43" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="10" spans="2:15" ht="157.5" customHeight="1">
-      <c r="B10" s="118" t="s">
-        <v>190</v>
-      </c>
-      <c r="C10" s="125" t="s">
-        <v>191</v>
-      </c>
-      <c r="E10" s="118" t="s">
-        <v>190</v>
-      </c>
-      <c r="F10" s="122" t="s">
-        <v>192</v>
+      <c r="B10" s="36" t="s">
+        <v>201</v>
+      </c>
+      <c r="C10" s="43" t="s">
+        <v>202</v>
+      </c>
+      <c r="E10" s="36" t="s">
+        <v>201</v>
+      </c>
+      <c r="F10" s="40" t="s">
+        <v>203</v>
       </c>
       <c r="G10" s="1"/>
-      <c r="H10" s="118" t="s">
-        <v>190</v>
-      </c>
-      <c r="I10" s="122" t="s">
-        <v>193</v>
+      <c r="H10" s="36" t="s">
+        <v>201</v>
+      </c>
+      <c r="I10" s="40" t="s">
+        <v>204</v>
       </c>
       <c r="J10" s="1"/>
-      <c r="K10" s="118" t="s">
-        <v>190</v>
-      </c>
-      <c r="L10" s="122" t="s">
-        <v>194</v>
+      <c r="K10" s="36" t="s">
+        <v>201</v>
+      </c>
+      <c r="L10" s="40" t="s">
+        <v>205</v>
       </c>
       <c r="M10" s="1"/>
-      <c r="N10" s="118" t="s">
-        <v>190</v>
-      </c>
-      <c r="O10" s="122" t="s">
-        <v>195</v>
+      <c r="N10" s="36" t="s">
+        <v>201</v>
+      </c>
+      <c r="O10" s="40" t="s">
+        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -6553,7 +7232,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25E0E957-9C5A-4452-A155-DBEDE045AA52}">
   <dimension ref="B1:I15"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="H10" sqref="H10:I15"/>
     </sheetView>
   </sheetViews>
@@ -6571,243 +7250,243 @@
     <row r="1" spans="2:9" ht="3.75" customHeight="1"/>
     <row r="2" spans="2:9" ht="6" customHeight="1"/>
     <row r="3" spans="2:9">
-      <c r="B3" s="118" t="s">
-        <v>153</v>
-      </c>
-      <c r="C3" s="119" t="s">
-        <v>196</v>
-      </c>
-      <c r="E3" s="118" t="s">
-        <v>153</v>
-      </c>
-      <c r="F3" s="119" t="s">
-        <v>197</v>
-      </c>
-      <c r="H3" s="118" t="s">
-        <v>153</v>
-      </c>
-      <c r="I3" s="119" t="s">
-        <v>198</v>
+      <c r="B3" s="36" t="s">
+        <v>164</v>
+      </c>
+      <c r="C3" s="37" t="s">
+        <v>207</v>
+      </c>
+      <c r="E3" s="36" t="s">
+        <v>164</v>
+      </c>
+      <c r="F3" s="37" t="s">
+        <v>208</v>
+      </c>
+      <c r="H3" s="36" t="s">
+        <v>164</v>
+      </c>
+      <c r="I3" s="37" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="4" spans="2:9" ht="89.25" customHeight="1">
-      <c r="B4" s="118" t="s">
-        <v>159</v>
-      </c>
-      <c r="C4" s="125" t="s">
-        <v>199</v>
-      </c>
-      <c r="E4" s="118" t="s">
-        <v>159</v>
-      </c>
-      <c r="F4" s="125" t="s">
-        <v>200</v>
-      </c>
-      <c r="H4" s="118" t="s">
-        <v>159</v>
-      </c>
-      <c r="I4" s="125" t="s">
-        <v>201</v>
+      <c r="B4" s="36" t="s">
+        <v>170</v>
+      </c>
+      <c r="C4" s="43" t="s">
+        <v>210</v>
+      </c>
+      <c r="E4" s="36" t="s">
+        <v>170</v>
+      </c>
+      <c r="F4" s="43" t="s">
+        <v>211</v>
+      </c>
+      <c r="H4" s="36" t="s">
+        <v>170</v>
+      </c>
+      <c r="I4" s="43" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="5" spans="2:9">
-      <c r="B5" s="118" t="s">
-        <v>165</v>
-      </c>
-      <c r="C5" s="124" t="s">
-        <v>166</v>
-      </c>
-      <c r="E5" s="118" t="s">
-        <v>165</v>
-      </c>
-      <c r="F5" s="124" t="s">
-        <v>166</v>
-      </c>
-      <c r="H5" s="118" t="s">
-        <v>165</v>
-      </c>
-      <c r="I5" s="124" t="s">
-        <v>166</v>
+      <c r="B5" s="36" t="s">
+        <v>176</v>
+      </c>
+      <c r="C5" s="42" t="s">
+        <v>177</v>
+      </c>
+      <c r="E5" s="36" t="s">
+        <v>176</v>
+      </c>
+      <c r="F5" s="42" t="s">
+        <v>177</v>
+      </c>
+      <c r="H5" s="36" t="s">
+        <v>176</v>
+      </c>
+      <c r="I5" s="42" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="6" spans="2:9">
-      <c r="B6" s="118" t="s">
-        <v>168</v>
-      </c>
-      <c r="C6" s="124" t="s">
-        <v>169</v>
-      </c>
-      <c r="E6" s="118" t="s">
-        <v>168</v>
-      </c>
-      <c r="F6" s="124" t="s">
-        <v>169</v>
-      </c>
-      <c r="H6" s="118" t="s">
-        <v>168</v>
-      </c>
-      <c r="I6" s="124" t="s">
-        <v>169</v>
+      <c r="B6" s="36" t="s">
+        <v>179</v>
+      </c>
+      <c r="C6" s="42" t="s">
+        <v>180</v>
+      </c>
+      <c r="E6" s="36" t="s">
+        <v>179</v>
+      </c>
+      <c r="F6" s="42" t="s">
+        <v>180</v>
+      </c>
+      <c r="H6" s="36" t="s">
+        <v>179</v>
+      </c>
+      <c r="I6" s="42" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="7" spans="2:9" ht="150" customHeight="1">
-      <c r="B7" s="118" t="s">
-        <v>178</v>
-      </c>
-      <c r="C7" s="125" t="s">
-        <v>202</v>
-      </c>
-      <c r="E7" s="118" t="s">
-        <v>178</v>
-      </c>
-      <c r="F7" s="125" t="s">
-        <v>203</v>
-      </c>
-      <c r="H7" s="118" t="s">
-        <v>178</v>
-      </c>
-      <c r="I7" s="125" t="s">
-        <v>204</v>
+      <c r="B7" s="36" t="s">
+        <v>189</v>
+      </c>
+      <c r="C7" s="43" t="s">
+        <v>213</v>
+      </c>
+      <c r="E7" s="36" t="s">
+        <v>189</v>
+      </c>
+      <c r="F7" s="43" t="s">
+        <v>214</v>
+      </c>
+      <c r="H7" s="36" t="s">
+        <v>189</v>
+      </c>
+      <c r="I7" s="43" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="8" spans="2:9" ht="72" customHeight="1">
-      <c r="B8" s="118" t="s">
-        <v>184</v>
-      </c>
-      <c r="C8" s="125" t="s">
-        <v>205</v>
-      </c>
-      <c r="E8" s="118" t="s">
-        <v>184</v>
-      </c>
-      <c r="F8" s="125" t="s">
-        <v>206</v>
-      </c>
-      <c r="H8" s="118" t="s">
-        <v>184</v>
-      </c>
-      <c r="I8" s="125" t="s">
-        <v>207</v>
+      <c r="B8" s="36" t="s">
+        <v>195</v>
+      </c>
+      <c r="C8" s="43" t="s">
+        <v>216</v>
+      </c>
+      <c r="E8" s="36" t="s">
+        <v>195</v>
+      </c>
+      <c r="F8" s="43" t="s">
+        <v>217</v>
+      </c>
+      <c r="H8" s="36" t="s">
+        <v>195</v>
+      </c>
+      <c r="I8" s="43" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="10" spans="2:9">
-      <c r="B10" s="118" t="s">
-        <v>153</v>
-      </c>
-      <c r="C10" s="119" t="s">
-        <v>208</v>
-      </c>
-      <c r="E10" s="118" t="s">
-        <v>153</v>
-      </c>
-      <c r="F10" s="119" t="s">
-        <v>209</v>
-      </c>
-      <c r="H10" s="118" t="s">
-        <v>153</v>
-      </c>
-      <c r="I10" s="119" t="s">
-        <v>210</v>
+      <c r="B10" s="36" t="s">
+        <v>164</v>
+      </c>
+      <c r="C10" s="37" t="s">
+        <v>219</v>
+      </c>
+      <c r="E10" s="36" t="s">
+        <v>164</v>
+      </c>
+      <c r="F10" s="37" t="s">
+        <v>220</v>
+      </c>
+      <c r="H10" s="36" t="s">
+        <v>164</v>
+      </c>
+      <c r="I10" s="37" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="11" spans="2:9" ht="68.25" customHeight="1">
-      <c r="B11" s="118" t="s">
-        <v>159</v>
-      </c>
-      <c r="C11" s="125" t="s">
-        <v>211</v>
-      </c>
-      <c r="E11" s="118" t="s">
-        <v>159</v>
-      </c>
-      <c r="F11" s="125" t="s">
-        <v>212</v>
-      </c>
-      <c r="H11" s="118" t="s">
-        <v>159</v>
-      </c>
-      <c r="I11" s="125" t="s">
-        <v>213</v>
+      <c r="B11" s="36" t="s">
+        <v>170</v>
+      </c>
+      <c r="C11" s="43" t="s">
+        <v>222</v>
+      </c>
+      <c r="E11" s="36" t="s">
+        <v>170</v>
+      </c>
+      <c r="F11" s="43" t="s">
+        <v>223</v>
+      </c>
+      <c r="H11" s="36" t="s">
+        <v>170</v>
+      </c>
+      <c r="I11" s="43" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="12" spans="2:9">
-      <c r="B12" s="118" t="s">
-        <v>165</v>
-      </c>
-      <c r="C12" s="124" t="s">
-        <v>166</v>
-      </c>
-      <c r="E12" s="118" t="s">
-        <v>165</v>
-      </c>
-      <c r="F12" s="124" t="s">
-        <v>166</v>
-      </c>
-      <c r="H12" s="118" t="s">
-        <v>165</v>
-      </c>
-      <c r="I12" s="124" t="s">
-        <v>166</v>
+      <c r="B12" s="36" t="s">
+        <v>176</v>
+      </c>
+      <c r="C12" s="42" t="s">
+        <v>177</v>
+      </c>
+      <c r="E12" s="36" t="s">
+        <v>176</v>
+      </c>
+      <c r="F12" s="42" t="s">
+        <v>177</v>
+      </c>
+      <c r="H12" s="36" t="s">
+        <v>176</v>
+      </c>
+      <c r="I12" s="42" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="13" spans="2:9">
-      <c r="B13" s="118" t="s">
-        <v>168</v>
-      </c>
-      <c r="C13" s="124" t="s">
-        <v>169</v>
-      </c>
-      <c r="E13" s="118" t="s">
-        <v>168</v>
-      </c>
-      <c r="F13" s="124" t="s">
-        <v>169</v>
-      </c>
-      <c r="H13" s="118" t="s">
-        <v>168</v>
-      </c>
-      <c r="I13" s="124" t="s">
-        <v>169</v>
+      <c r="B13" s="36" t="s">
+        <v>179</v>
+      </c>
+      <c r="C13" s="42" t="s">
+        <v>180</v>
+      </c>
+      <c r="E13" s="36" t="s">
+        <v>179</v>
+      </c>
+      <c r="F13" s="42" t="s">
+        <v>180</v>
+      </c>
+      <c r="H13" s="36" t="s">
+        <v>179</v>
+      </c>
+      <c r="I13" s="42" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="14" spans="2:9" ht="171" customHeight="1">
-      <c r="B14" s="118" t="s">
-        <v>178</v>
-      </c>
-      <c r="C14" s="125" t="s">
-        <v>214</v>
-      </c>
-      <c r="E14" s="118" t="s">
-        <v>178</v>
-      </c>
-      <c r="F14" s="125" t="s">
-        <v>215</v>
-      </c>
-      <c r="H14" s="118" t="s">
-        <v>178</v>
-      </c>
-      <c r="I14" s="125" t="s">
-        <v>216</v>
+      <c r="B14" s="36" t="s">
+        <v>189</v>
+      </c>
+      <c r="C14" s="43" t="s">
+        <v>225</v>
+      </c>
+      <c r="E14" s="36" t="s">
+        <v>189</v>
+      </c>
+      <c r="F14" s="43" t="s">
+        <v>226</v>
+      </c>
+      <c r="H14" s="36" t="s">
+        <v>189</v>
+      </c>
+      <c r="I14" s="43" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="15" spans="2:9" ht="45.75">
-      <c r="B15" s="118" t="s">
-        <v>184</v>
-      </c>
-      <c r="C15" s="125" t="s">
-        <v>217</v>
-      </c>
-      <c r="E15" s="118" t="s">
-        <v>184</v>
-      </c>
-      <c r="F15" s="125" t="s">
-        <v>218</v>
-      </c>
-      <c r="H15" s="118" t="s">
-        <v>184</v>
-      </c>
-      <c r="I15" s="125" t="s">
-        <v>219</v>
+      <c r="B15" s="36" t="s">
+        <v>195</v>
+      </c>
+      <c r="C15" s="43" t="s">
+        <v>228</v>
+      </c>
+      <c r="E15" s="36" t="s">
+        <v>195</v>
+      </c>
+      <c r="F15" s="43" t="s">
+        <v>229</v>
+      </c>
+      <c r="H15" s="36" t="s">
+        <v>195</v>
+      </c>
+      <c r="I15" s="43" t="s">
+        <v>230</v>
       </c>
     </row>
   </sheetData>
@@ -6820,7 +7499,7 @@
   <dimension ref="B2:M5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6839,122 +7518,117 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:13" ht="18">
-      <c r="B2" s="127" t="s">
-        <v>220</v>
-      </c>
-      <c r="C2" s="127"/>
-      <c r="D2" s="127"/>
-      <c r="E2" s="127"/>
-      <c r="F2" s="127"/>
-      <c r="G2" s="127"/>
-      <c r="H2" s="127"/>
-      <c r="I2" s="127"/>
-      <c r="J2" s="127"/>
-      <c r="K2" s="127"/>
-      <c r="L2" s="127"/>
-      <c r="M2" s="127"/>
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
+      <c r="J2" s="84"/>
+      <c r="K2" s="84"/>
+      <c r="L2" s="84"/>
+      <c r="M2" s="84"/>
     </row>
     <row r="3" spans="2:13" ht="57.75" customHeight="1">
-      <c r="B3" s="128" t="s">
-        <v>221</v>
-      </c>
-      <c r="C3" s="128" t="s">
-        <v>222</v>
-      </c>
-      <c r="D3" s="128" t="s">
-        <v>223</v>
-      </c>
-      <c r="E3" s="128" t="s">
-        <v>224</v>
-      </c>
-      <c r="F3" s="128" t="s">
-        <v>225</v>
-      </c>
-      <c r="G3" s="128" t="s">
-        <v>226</v>
-      </c>
-      <c r="H3" s="128" t="s">
-        <v>227</v>
-      </c>
-      <c r="I3" s="128" t="s">
-        <v>228</v>
-      </c>
-      <c r="J3" s="130" t="s">
-        <v>165</v>
-      </c>
-      <c r="K3" s="128" t="s">
-        <v>229</v>
-      </c>
-      <c r="L3" s="132"/>
+      <c r="B3" s="45" t="s">
+        <v>231</v>
+      </c>
+      <c r="C3" s="45" t="s">
+        <v>232</v>
+      </c>
+      <c r="D3" s="45" t="s">
+        <v>233</v>
+      </c>
+      <c r="E3" s="45" t="s">
+        <v>234</v>
+      </c>
+      <c r="F3" s="45" t="s">
+        <v>235</v>
+      </c>
+      <c r="G3" s="45" t="s">
+        <v>236</v>
+      </c>
+      <c r="H3" s="45" t="s">
+        <v>237</v>
+      </c>
+      <c r="I3" s="45" t="s">
+        <v>238</v>
+      </c>
+      <c r="J3" s="47" t="s">
+        <v>176</v>
+      </c>
+      <c r="K3" s="45" t="s">
+        <v>239</v>
+      </c>
+      <c r="L3" s="83"/>
     </row>
     <row r="4" spans="2:13" ht="91.5">
-      <c r="B4" s="123">
+      <c r="B4" s="41">
         <v>1</v>
       </c>
-      <c r="C4" s="123" t="s">
-        <v>230</v>
-      </c>
-      <c r="D4" s="125" t="s">
-        <v>231</v>
-      </c>
-      <c r="E4" s="123" t="s">
-        <v>232</v>
-      </c>
-      <c r="F4" s="129">
+      <c r="C4" s="41" t="s">
+        <v>240</v>
+      </c>
+      <c r="D4" s="43" t="s">
+        <v>241</v>
+      </c>
+      <c r="E4" s="41" t="s">
+        <v>242</v>
+      </c>
+      <c r="F4" s="46">
         <v>44979</v>
       </c>
-      <c r="G4" s="123" t="s">
-        <v>233</v>
-      </c>
-      <c r="H4" s="123" t="s">
-        <v>234</v>
-      </c>
-      <c r="I4" s="123" t="s">
-        <v>166</v>
-      </c>
-      <c r="J4" s="123" t="s">
-        <v>166</v>
-      </c>
-      <c r="K4" s="131" t="s">
-        <v>235</v>
+      <c r="G4" s="41" t="s">
+        <v>243</v>
+      </c>
+      <c r="H4" s="41" t="s">
+        <v>244</v>
+      </c>
+      <c r="I4" s="41" t="s">
+        <v>177</v>
+      </c>
+      <c r="J4" s="41" t="s">
+        <v>177</v>
+      </c>
+      <c r="K4" s="48" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="5" spans="2:13" ht="76.5">
-      <c r="B5" s="123">
+      <c r="B5" s="41">
         <v>2</v>
       </c>
-      <c r="C5" s="123" t="s">
-        <v>236</v>
-      </c>
-      <c r="D5" s="125" t="s">
-        <v>237</v>
-      </c>
-      <c r="E5" s="123" t="s">
-        <v>232</v>
-      </c>
-      <c r="F5" s="129">
+      <c r="C5" s="41" t="s">
+        <v>246</v>
+      </c>
+      <c r="D5" s="43" t="s">
+        <v>247</v>
+      </c>
+      <c r="E5" s="41" t="s">
+        <v>242</v>
+      </c>
+      <c r="F5" s="46">
         <v>44979</v>
       </c>
-      <c r="G5" s="123" t="s">
-        <v>233</v>
-      </c>
-      <c r="H5" s="123" t="s">
-        <v>234</v>
-      </c>
-      <c r="I5" s="123" t="s">
-        <v>238</v>
-      </c>
-      <c r="J5" s="123" t="s">
-        <v>166</v>
-      </c>
-      <c r="K5" s="123" t="s">
-        <v>235</v>
+      <c r="G5" s="41" t="s">
+        <v>243</v>
+      </c>
+      <c r="H5" s="41" t="s">
+        <v>244</v>
+      </c>
+      <c r="I5" s="41" t="s">
+        <v>248</v>
+      </c>
+      <c r="J5" s="41" t="s">
+        <v>177</v>
+      </c>
+      <c r="K5" s="41" t="s">
+        <v>245</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B2:M2"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ajuste de estrategia, restricciones y mitigación riesgos
</commit_message>
<xml_diff>
--- a/ESTRATEGIA(PROCESO DE PRUEBAS).xlsx
+++ b/ESTRATEGIA(PROCESO DE PRUEBAS).xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26216"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26220"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="1560" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3367A073-DDAD-49BE-9600-D8DB02DF0751}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B9B6EE45-69BB-498F-876C-FDB24EC5BD65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VISIÓN" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="251">
   <si>
     <t xml:space="preserve">Check List </t>
   </si>
@@ -327,7 +327,7 @@
   </si>
   <si>
     <r>
-      <t>2</t>
+      <t>Plan de pruebas general</t>
     </r>
     <r>
       <rPr>
@@ -340,8 +340,11 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>3</t>
+    <t> </t>
+  </si>
+  <si>
+    <r>
+      <t>Logística</t>
     </r>
     <r>
       <rPr>
@@ -355,7 +358,7 @@
   </si>
   <si>
     <r>
-      <t>Plan de pruebas general</t>
+      <t>Asignación de rol analistas</t>
     </r>
     <r>
       <rPr>
@@ -369,7 +372,7 @@
   </si>
   <si>
     <r>
-      <t>1</t>
+      <t>Ceremonias SCRUM</t>
     </r>
     <r>
       <rPr>
@@ -383,7 +386,7 @@
   </si>
   <si>
     <r>
-      <t>4</t>
+      <t>Planteamiento Herramienta de pruebas</t>
     </r>
     <r>
       <rPr>
@@ -396,11 +399,8 @@
     </r>
   </si>
   <si>
-    <t> </t>
-  </si>
-  <si>
-    <r>
-      <t>Logística</t>
+    <r>
+      <t>Verificación de datos</t>
     </r>
     <r>
       <rPr>
@@ -414,7 +414,7 @@
   </si>
   <si>
     <r>
-      <t>Asignación de rol analistas</t>
+      <t>Preparaciones ambientes</t>
     </r>
     <r>
       <rPr>
@@ -428,7 +428,7 @@
   </si>
   <si>
     <r>
-      <t>Ceremonias SCRUM</t>
+      <t>Planeación</t>
     </r>
     <r>
       <rPr>
@@ -442,7 +442,7 @@
   </si>
   <si>
     <r>
-      <t>7</t>
+      <t>Cronograma de actividades</t>
     </r>
     <r>
       <rPr>
@@ -456,7 +456,7 @@
   </si>
   <si>
     <r>
-      <t>1,5</t>
+      <t>Plan detallado de pruebas</t>
     </r>
     <r>
       <rPr>
@@ -470,7 +470,7 @@
   </si>
   <si>
     <r>
-      <t>Planteamiento Herramienta de pruebas</t>
+      <t>Reunión aprobación</t>
     </r>
     <r>
       <rPr>
@@ -484,7 +484,7 @@
   </si>
   <si>
     <r>
-      <t>Verificación de datos</t>
+      <t>Diseño</t>
     </r>
     <r>
       <rPr>
@@ -498,7 +498,7 @@
   </si>
   <si>
     <r>
-      <t>Preparaciones ambientes</t>
+      <t>Pruebas funcionales - Riesgos</t>
     </r>
     <r>
       <rPr>
@@ -512,7 +512,7 @@
   </si>
   <si>
     <r>
-      <t>Planeación</t>
+      <t>Pruebas de Usabilidad - Riesgos</t>
     </r>
     <r>
       <rPr>
@@ -526,7 +526,7 @@
   </si>
   <si>
     <r>
-      <t>Cronograma de actividades</t>
+      <t>Pruebas de Rendimiento - Riesgos</t>
     </r>
     <r>
       <rPr>
@@ -540,7 +540,7 @@
   </si>
   <si>
     <r>
-      <t>Plan detallado de pruebas</t>
+      <t>Ejecución</t>
     </r>
     <r>
       <rPr>
@@ -554,7 +554,7 @@
   </si>
   <si>
     <r>
-      <t>Reunión aprobación</t>
+      <t>Pruebas exploratorias</t>
     </r>
     <r>
       <rPr>
@@ -567,8 +567,11 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>Diseño</t>
+    <t>smoke test</t>
+  </si>
+  <si>
+    <r>
+      <t>Pruebas Casos de uso</t>
     </r>
     <r>
       <rPr>
@@ -582,7 +585,7 @@
   </si>
   <si>
     <r>
-      <t>Pruebas funcionales - Riesgos</t>
+      <t>Transición de Estados</t>
     </r>
     <r>
       <rPr>
@@ -596,7 +599,7 @@
   </si>
   <si>
     <r>
-      <t>6</t>
+      <t>Usabilidad</t>
     </r>
     <r>
       <rPr>
@@ -610,7 +613,7 @@
   </si>
   <si>
     <r>
-      <t>5</t>
+      <t>Pruebas de Rendimiento</t>
     </r>
     <r>
       <rPr>
@@ -623,8 +626,11 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>Pruebas de Usabilidad - Riesgos</t>
+    <t>Gestión</t>
+  </si>
+  <si>
+    <r>
+      <t>Reporte de issues</t>
     </r>
     <r>
       <rPr>
@@ -638,7 +644,7 @@
   </si>
   <si>
     <r>
-      <t>Pruebas de Rendimiento - Riesgos</t>
+      <t>Gestión de issues</t>
     </r>
     <r>
       <rPr>
@@ -652,7 +658,7 @@
   </si>
   <si>
     <r>
-      <t>Ejecución</t>
+      <t>Entrega de prueba</t>
     </r>
     <r>
       <rPr>
@@ -666,7 +672,7 @@
   </si>
   <si>
     <r>
-      <t>Pruebas exploratorias</t>
+      <t>Informe resultados pruebas</t>
     </r>
     <r>
       <rPr>
@@ -679,11 +685,8 @@
     </r>
   </si>
   <si>
-    <t>smoke test</t>
-  </si>
-  <si>
-    <r>
-      <t>Pruebas Casos de uso</t>
+    <r>
+      <t>Esfuerzo estimado</t>
     </r>
     <r>
       <rPr>
@@ -697,7 +700,7 @@
   </si>
   <si>
     <r>
-      <t>Transición de Estados</t>
+      <t>Factor de ajuste</t>
     </r>
     <r>
       <rPr>
@@ -711,7 +714,7 @@
   </si>
   <si>
     <r>
-      <t>Usabilidad</t>
+      <t>Horas total analista x día</t>
     </r>
     <r>
       <rPr>
@@ -725,7 +728,7 @@
   </si>
   <si>
     <r>
-      <t>Pruebas de Rendimiento</t>
+      <t>Esfuerzo más probable</t>
     </r>
     <r>
       <rPr>
@@ -738,11 +741,8 @@
     </r>
   </si>
   <si>
-    <t>Gestión</t>
-  </si>
-  <si>
-    <r>
-      <t>Reporte de issues</t>
+    <r>
+      <t>Total de dia de dias pesimistas </t>
     </r>
     <r>
       <rPr>
@@ -756,7 +756,7 @@
   </si>
   <si>
     <r>
-      <t>Gestión de issues</t>
+      <t>3 personas se gastan </t>
     </r>
     <r>
       <rPr>
@@ -770,7 +770,7 @@
   </si>
   <si>
     <r>
-      <t>Entrega de prueba</t>
+      <t>Días </t>
     </r>
     <r>
       <rPr>
@@ -783,132 +783,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>Informe resultados pruebas</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <charset val="1"/>
-      </rPr>
-      <t> </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Esfuerzo estimado</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <charset val="1"/>
-      </rPr>
-      <t> </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Factor de ajuste</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <charset val="1"/>
-      </rPr>
-      <t> </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Horas total analista x día</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <charset val="1"/>
-      </rPr>
-      <t> </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Esfuerzo más probable</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <charset val="1"/>
-      </rPr>
-      <t> </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Total de dia de dias pesimistas </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <charset val="1"/>
-      </rPr>
-      <t> </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>3 personas se gastan </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <charset val="1"/>
-      </rPr>
-      <t> </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Días </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <charset val="1"/>
-      </rPr>
-      <t> </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>4,7</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <charset val="1"/>
-      </rPr>
-      <t> </t>
-    </r>
-  </si>
-  <si>
     <t>1. Identificar</t>
   </si>
   <si>
@@ -937,6 +811,9 @@
   </si>
   <si>
     <t>Plan de Accion o Mitigación</t>
+  </si>
+  <si>
+    <t>33% ch</t>
   </si>
   <si>
     <t>Planificación incorrecta</t>
@@ -1026,8 +903,8 @@
     <t>La funcion de consultar cursos, no sea posible de hacerse con ningun curso.</t>
   </si>
   <si>
-    <t>Realizar pruebas de partición de equivalencias
-Pruebas de sistema</t>
+    <t>Smoke test
+Pruebas de componente</t>
   </si>
   <si>
     <t>Fallas al interactuar con los elementos del aplicativo</t>
@@ -1117,6 +994,36 @@
     <t>&gt;Pruebas de Rendimiento
 &gt;Pruebas Exploratorias
 &gt;Pruebas de Transición de estados</t>
+  </si>
+  <si>
+    <t>RESTRICCIONES</t>
+  </si>
+  <si>
+    <t>FIJO</t>
+  </si>
+  <si>
+    <t>DESEADO</t>
+  </si>
+  <si>
+    <t>AJUSTABLE</t>
+  </si>
+  <si>
+    <t>Analistas asignados</t>
+  </si>
+  <si>
+    <t>Una Funcionalidad</t>
+  </si>
+  <si>
+    <t>Tiempo de Entrega</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alcance de pruebas </t>
+  </si>
+  <si>
+    <t>Recuersos de herramientas testing</t>
+  </si>
+  <si>
+    <t>Plataforma Del Aplicativo</t>
   </si>
   <si>
     <t>ID</t>
@@ -1446,7 +1353,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1569,8 +1476,14 @@
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="15">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1655,6 +1568,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="32">
     <border>
@@ -2009,7 +1934,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="139">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2147,125 +2072,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2274,7 +2097,7 @@
     <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2289,55 +2112,19 @@
     <xf numFmtId="0" fontId="19" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="10" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="1" fontId="10" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2348,20 +2135,198 @@
     <xf numFmtId="9" fontId="10" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="21" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="10" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4864,6 +4829,347 @@
         <a:xfrm>
           <a:off x="4972050" y="5372100"/>
           <a:ext cx="183375" cy="183375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>609601</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>19051</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1" descr="Marca de verificación">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C6931FD-D506-4AFA-97B7-25CFECF5E23E}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{9BB2DB53-CE87-4B86-A5EC-C1C6B201CE2F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1781175" y="5162550"/>
+          <a:ext cx="219076" cy="219076"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>609601</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>9526</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2" descr="Marca de verificación">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4D745570-AA64-40C0-8699-CEBF50B7016F}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{9C6931FD-D506-4AFA-97B7-25CFECF5E23E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1781175" y="5343525"/>
+          <a:ext cx="219076" cy="219076"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1000125</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1219201</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>28576</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagen 3" descr="Marca de verificación">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E6D7C66F-689C-454A-BCD7-61FEFC395393}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{4D745570-AA64-40C0-8699-CEBF50B7016F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3067050" y="5553075"/>
+          <a:ext cx="219076" cy="219076"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>609601</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Imagen 4" descr="Marca de verificación">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{64551C35-8E48-43FB-9B6C-A42F0732F8B9}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{E6D7C66F-689C-454A-BCD7-61FEFC395393}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1781175" y="5715000"/>
+          <a:ext cx="219076" cy="219076"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>609601</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>266701</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Imagen 5" descr="Marca de verificación">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB0ACFDA-F7A9-470D-8EF1-226E69D2279B}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{64551C35-8E48-43FB-9B6C-A42F0732F8B9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1781175" y="6343650"/>
+          <a:ext cx="219076" cy="219076"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>609601</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>276226</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Imagen 6" descr="Marca de verificación">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3EC756F5-3FC1-429C-9FE1-3480EE8D7C5C}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{EB0ACFDA-F7A9-470D-8EF1-226E69D2279B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1781175" y="5991225"/>
+          <a:ext cx="219076" cy="219076"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5209,14 +5515,14 @@
   </cols>
   <sheetData>
     <row r="3" spans="4:10" ht="15.75">
-      <c r="D3" s="49" t="s">
+      <c r="D3" s="84" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="49"/>
-      <c r="F3" s="49"/>
-      <c r="G3" s="49"/>
-      <c r="H3" s="49"/>
-      <c r="I3" s="49"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="84"/>
+      <c r="G3" s="84"/>
+      <c r="H3" s="84"/>
+      <c r="I3" s="84"/>
       <c r="J3" s="4"/>
     </row>
     <row r="4" spans="4:10" ht="15.75">
@@ -5602,20 +5908,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:10">
-      <c r="C1" s="52" t="s">
+      <c r="C1" s="87" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="87"/>
+      <c r="G1" s="87"/>
     </row>
     <row r="2" spans="2:10" ht="7.5" customHeight="1">
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
+      <c r="C2" s="87"/>
+      <c r="D2" s="87"/>
+      <c r="E2" s="87"/>
+      <c r="F2" s="87"/>
+      <c r="G2" s="87"/>
     </row>
     <row r="3" spans="2:10" ht="21.75" customHeight="1">
       <c r="B3" s="1"/>
@@ -5638,49 +5944,49 @@
       <c r="J3" s="1"/>
     </row>
     <row r="4" spans="2:10" ht="186" customHeight="1">
-      <c r="C4" s="50" t="s">
+      <c r="C4" s="85" t="s">
         <v>46</v>
       </c>
-      <c r="D4" s="55" t="s">
+      <c r="D4" s="90" t="s">
         <v>47</v>
       </c>
-      <c r="E4" s="53" t="s">
+      <c r="E4" s="88" t="s">
         <v>48</v>
       </c>
-      <c r="F4" s="53" t="s">
+      <c r="F4" s="88" t="s">
         <v>49</v>
       </c>
-      <c r="G4" s="51" t="s">
+      <c r="G4" s="86" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="5" spans="2:10">
-      <c r="C5" s="50"/>
-      <c r="D5" s="56"/>
-      <c r="E5" s="54"/>
-      <c r="F5" s="54"/>
-      <c r="G5" s="51"/>
+      <c r="C5" s="85"/>
+      <c r="D5" s="91"/>
+      <c r="E5" s="89"/>
+      <c r="F5" s="89"/>
+      <c r="G5" s="86"/>
     </row>
     <row r="6" spans="2:10">
-      <c r="C6" s="50"/>
-      <c r="D6" s="56"/>
-      <c r="E6" s="54"/>
-      <c r="F6" s="54"/>
-      <c r="G6" s="51"/>
+      <c r="C6" s="85"/>
+      <c r="D6" s="91"/>
+      <c r="E6" s="89"/>
+      <c r="F6" s="89"/>
+      <c r="G6" s="86"/>
     </row>
     <row r="7" spans="2:10">
-      <c r="C7" s="50"/>
-      <c r="D7" s="56"/>
-      <c r="E7" s="54"/>
-      <c r="F7" s="54"/>
-      <c r="G7" s="51"/>
+      <c r="C7" s="85"/>
+      <c r="D7" s="91"/>
+      <c r="E7" s="89"/>
+      <c r="F7" s="89"/>
+      <c r="G7" s="86"/>
     </row>
     <row r="8" spans="2:10" ht="201.75" customHeight="1">
-      <c r="C8" s="50"/>
-      <c r="D8" s="56"/>
-      <c r="E8" s="54"/>
-      <c r="F8" s="54"/>
-      <c r="G8" s="51"/>
+      <c r="C8" s="85"/>
+      <c r="D8" s="91"/>
+      <c r="E8" s="89"/>
+      <c r="F8" s="89"/>
+      <c r="G8" s="86"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -5700,14 +6006,14 @@
   <dimension ref="D1:K39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="R24" sqref="R24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="1.7109375" customWidth="1"/>
     <col min="4" max="4" width="17.42578125" customWidth="1"/>
-    <col min="5" max="5" width="28" customWidth="1"/>
+    <col min="5" max="5" width="31.28515625" customWidth="1"/>
     <col min="6" max="6" width="12.5703125" customWidth="1"/>
     <col min="7" max="7" width="16" customWidth="1"/>
     <col min="8" max="8" width="14.85546875" customWidth="1"/>
@@ -5716,583 +6022,594 @@
     <row r="1" spans="4:11" ht="6.75" customHeight="1"/>
     <row r="2" spans="4:11" ht="0.75" customHeight="1"/>
     <row r="3" spans="4:11">
-      <c r="D3" s="98" t="s">
+      <c r="D3" s="96" t="s">
         <v>51</v>
       </c>
-      <c r="E3" s="99"/>
-      <c r="F3" s="85" t="s">
+      <c r="E3" s="97"/>
+      <c r="F3" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="G3" s="85" t="s">
+      <c r="G3" s="51" t="s">
         <v>53</v>
       </c>
-      <c r="H3" s="85" t="s">
+      <c r="H3" s="77" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="4" spans="4:11" ht="13.5" customHeight="1">
-      <c r="D4" s="102" t="s">
+      <c r="D4" s="95" t="s">
         <v>55</v>
       </c>
-      <c r="E4" s="86" t="s">
+      <c r="E4" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="F4" s="119" t="s">
+      <c r="F4" s="72">
+        <v>2</v>
+      </c>
+      <c r="G4" s="72">
+        <v>3</v>
+      </c>
+      <c r="H4" s="76">
+        <f>(F4*G4)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="4:11" ht="16.5" customHeight="1">
+      <c r="D5" s="92"/>
+      <c r="E5" s="52" t="s">
         <v>57</v>
       </c>
-      <c r="G4" s="119" t="s">
+      <c r="F5" s="65">
+        <v>1</v>
+      </c>
+      <c r="G5" s="64">
+        <v>4</v>
+      </c>
+      <c r="H5" s="78">
+        <f>(F5*G5)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="4:11">
+      <c r="D6" s="54" t="s">
         <v>58</v>
       </c>
-      <c r="H4" s="113">
+      <c r="E6" s="55" t="s">
+        <v>58</v>
+      </c>
+      <c r="F6" s="73" t="s">
+        <v>58</v>
+      </c>
+      <c r="G6" s="73" t="s">
+        <v>58</v>
+      </c>
+      <c r="H6" s="69" t="s">
+        <v>58</v>
+      </c>
+      <c r="K6" s="7"/>
+    </row>
+    <row r="7" spans="4:11" ht="16.5" customHeight="1">
+      <c r="D7" s="94" t="s">
+        <v>59</v>
+      </c>
+      <c r="E7" s="52" t="s">
+        <v>60</v>
+      </c>
+      <c r="F7" s="65">
+        <v>1</v>
+      </c>
+      <c r="G7" s="65">
+        <v>3</v>
+      </c>
+      <c r="H7" s="78">
+        <f>(F7*G7)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="4:11" ht="17.25" customHeight="1">
+      <c r="D8" s="94"/>
+      <c r="E8" s="52" t="s">
+        <v>61</v>
+      </c>
+      <c r="F8" s="65">
+        <v>7</v>
+      </c>
+      <c r="G8" s="65">
+        <v>1.5</v>
+      </c>
+      <c r="H8" s="82">
+        <f>(F8*G8)</f>
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="9" spans="4:11" ht="27" customHeight="1">
+      <c r="D9" s="94"/>
+      <c r="E9" s="52" t="s">
+        <v>62</v>
+      </c>
+      <c r="F9" s="65">
+        <v>1</v>
+      </c>
+      <c r="G9" s="65">
+        <v>3</v>
+      </c>
+      <c r="H9" s="68">
+        <f t="shared" ref="H9:H17" si="0">(F9*G9)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="4:11" ht="19.5" customHeight="1">
+      <c r="D10" s="94"/>
+      <c r="E10" s="52" t="s">
+        <v>63</v>
+      </c>
+      <c r="F10" s="65">
+        <v>1</v>
+      </c>
+      <c r="G10" s="65">
+        <v>2</v>
+      </c>
+      <c r="H10" s="68">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="4:11" ht="14.25" customHeight="1">
+      <c r="D11" s="94"/>
+      <c r="E11" s="52" t="s">
+        <v>64</v>
+      </c>
+      <c r="F11" s="65">
+        <v>1</v>
+      </c>
+      <c r="G11" s="65">
+        <v>3</v>
+      </c>
+      <c r="H11" s="68">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="4:11">
+      <c r="D12" s="63" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" s="55" t="s">
+        <v>58</v>
+      </c>
+      <c r="F12" s="73" t="s">
+        <v>58</v>
+      </c>
+      <c r="G12" s="73" t="s">
+        <v>58</v>
+      </c>
+      <c r="H12" s="69" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="4:11">
+      <c r="D13" s="94" t="s">
+        <v>65</v>
+      </c>
+      <c r="E13" s="52" t="s">
+        <v>66</v>
+      </c>
+      <c r="F13" s="65">
+        <v>1</v>
+      </c>
+      <c r="G13" s="65">
+        <v>3</v>
+      </c>
+      <c r="H13" s="68">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="4:11" ht="28.5" customHeight="1">
+      <c r="D14" s="94"/>
+      <c r="E14" s="75" t="s">
+        <v>67</v>
+      </c>
+      <c r="F14" s="65">
+        <v>1</v>
+      </c>
+      <c r="G14" s="65">
+        <v>4</v>
+      </c>
+      <c r="H14" s="68">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="4:11" ht="11.25" customHeight="1">
+      <c r="D15" s="94"/>
+      <c r="E15" s="52" t="s">
+        <v>68</v>
+      </c>
+      <c r="F15" s="65">
+        <v>1</v>
+      </c>
+      <c r="G15" s="65">
+        <v>2</v>
+      </c>
+      <c r="H15" s="68">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="4:11">
+      <c r="D16" s="54" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" s="55" t="s">
+        <v>58</v>
+      </c>
+      <c r="F16" s="73" t="s">
+        <v>58</v>
+      </c>
+      <c r="G16" s="73" t="s">
+        <v>58</v>
+      </c>
+      <c r="H16" s="69" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="4:8" ht="15" customHeight="1">
+      <c r="D17" s="94" t="s">
+        <v>69</v>
+      </c>
+      <c r="E17" s="52" t="s">
+        <v>70</v>
+      </c>
+      <c r="F17" s="65">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="4:11" ht="16.5" customHeight="1">
-      <c r="D5" s="103"/>
-      <c r="E5" s="86" t="s">
-        <v>59</v>
-      </c>
-      <c r="F5" s="120" t="s">
-        <v>60</v>
-      </c>
-      <c r="G5" s="121" t="s">
-        <v>61</v>
-      </c>
-      <c r="H5" s="114">
+      <c r="G17" s="65">
+        <v>5</v>
+      </c>
+      <c r="H17" s="68">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="4:8" ht="17.25" customHeight="1">
+      <c r="D18" s="94"/>
+      <c r="E18" s="79" t="s">
+        <v>71</v>
+      </c>
+      <c r="F18" s="65">
+        <v>2</v>
+      </c>
+      <c r="G18" s="65">
+        <v>3</v>
+      </c>
+      <c r="H18" s="68">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="4:8" ht="18.75" customHeight="1">
+      <c r="D19" s="94"/>
+      <c r="E19" s="74" t="s">
+        <v>72</v>
+      </c>
+      <c r="F19" s="65">
+        <v>3</v>
+      </c>
+      <c r="G19" s="65">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="4:11">
-      <c r="D6" s="88" t="s">
-        <v>62</v>
-      </c>
-      <c r="E6" s="89" t="s">
-        <v>62</v>
-      </c>
-      <c r="F6" s="122" t="s">
-        <v>62</v>
-      </c>
-      <c r="G6" s="122" t="s">
-        <v>62</v>
-      </c>
-      <c r="H6" s="115" t="s">
-        <v>62</v>
-      </c>
-      <c r="K6" s="7"/>
-    </row>
-    <row r="7" spans="4:11" ht="16.5" customHeight="1">
-      <c r="D7" s="100" t="s">
-        <v>63</v>
-      </c>
-      <c r="E7" s="86" t="s">
-        <v>64</v>
-      </c>
-      <c r="F7" s="120" t="s">
-        <v>60</v>
-      </c>
-      <c r="G7" s="120" t="s">
+      <c r="H19" s="68">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="4:8">
+      <c r="D20" s="54" t="s">
         <v>58</v>
       </c>
-      <c r="H7" s="114">
+      <c r="E20" s="55" t="s">
+        <v>58</v>
+      </c>
+      <c r="F20" s="73" t="s">
+        <v>58</v>
+      </c>
+      <c r="G20" s="73" t="s">
+        <v>58</v>
+      </c>
+      <c r="H20" s="69" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="4:8" ht="13.5" customHeight="1">
+      <c r="D21" s="102" t="s">
+        <v>73</v>
+      </c>
+      <c r="E21" s="52" t="s">
+        <v>74</v>
+      </c>
+      <c r="F21" s="65">
+        <v>2</v>
+      </c>
+      <c r="G21" s="65">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="4:11" ht="17.25" customHeight="1">
-      <c r="D8" s="100"/>
-      <c r="E8" s="86" t="s">
-        <v>65</v>
-      </c>
-      <c r="F8" s="120" t="s">
-        <v>66</v>
-      </c>
-      <c r="G8" s="120" t="s">
-        <v>67</v>
-      </c>
-      <c r="H8" s="114">
-        <v>10.5</v>
-      </c>
-    </row>
-    <row r="9" spans="4:11" ht="27" customHeight="1">
-      <c r="D9" s="100"/>
-      <c r="E9" s="86" t="s">
-        <v>68</v>
-      </c>
-      <c r="F9" s="120" t="s">
-        <v>60</v>
-      </c>
-      <c r="G9" s="120" t="s">
+      <c r="H21" s="68">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="4:8" ht="13.5" customHeight="1">
+      <c r="D22" s="102"/>
+      <c r="E22" s="52" t="s">
+        <v>75</v>
+      </c>
+      <c r="F22" s="65">
+        <v>2</v>
+      </c>
+      <c r="G22" s="65">
+        <v>3</v>
+      </c>
+      <c r="H22" s="68">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="4:8">
+      <c r="D23" s="102"/>
+      <c r="E23" s="53" t="s">
+        <v>76</v>
+      </c>
+      <c r="F23" s="65">
+        <v>3</v>
+      </c>
+      <c r="G23" s="65">
+        <v>5</v>
+      </c>
+      <c r="H23" s="68">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="4:8">
+      <c r="D24" s="102"/>
+      <c r="E24" s="52" t="s">
+        <v>77</v>
+      </c>
+      <c r="F24" s="65">
+        <v>2</v>
+      </c>
+      <c r="G24" s="65">
+        <v>3</v>
+      </c>
+      <c r="H24" s="68">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="4:8">
+      <c r="D25" s="102"/>
+      <c r="E25" s="52" t="s">
+        <v>78</v>
+      </c>
+      <c r="F25" s="65">
+        <v>2</v>
+      </c>
+      <c r="G25" s="65">
+        <v>3</v>
+      </c>
+      <c r="H25" s="68">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="4:8" ht="15.75" customHeight="1">
+      <c r="D26" s="102"/>
+      <c r="E26" s="53" t="s">
+        <v>79</v>
+      </c>
+      <c r="F26" s="65">
+        <v>2</v>
+      </c>
+      <c r="G26" s="65">
+        <v>4</v>
+      </c>
+      <c r="H26" s="68">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="4:8" ht="15.75" customHeight="1">
+      <c r="D27" s="54" t="s">
         <v>58</v>
       </c>
-      <c r="H9" s="114">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="4:11" ht="19.5" customHeight="1">
-      <c r="D10" s="100"/>
-      <c r="E10" s="86" t="s">
-        <v>69</v>
-      </c>
-      <c r="F10" s="120" t="s">
-        <v>60</v>
-      </c>
-      <c r="G10" s="120" t="s">
-        <v>57</v>
-      </c>
-      <c r="H10" s="114">
+      <c r="E27" s="55" t="s">
+        <v>58</v>
+      </c>
+      <c r="F27" s="73" t="s">
+        <v>58</v>
+      </c>
+      <c r="G27" s="73" t="s">
+        <v>58</v>
+      </c>
+      <c r="H27" s="69" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" spans="4:8" ht="15.75" customHeight="1">
+      <c r="D28" s="98" t="s">
+        <v>80</v>
+      </c>
+      <c r="E28" s="52" t="s">
+        <v>81</v>
+      </c>
+      <c r="F28" s="65">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="4:11" ht="14.25" customHeight="1">
-      <c r="D11" s="100"/>
-      <c r="E11" s="86" t="s">
-        <v>70</v>
-      </c>
-      <c r="F11" s="120" t="s">
-        <v>60</v>
-      </c>
-      <c r="G11" s="120" t="s">
+      <c r="G28" s="65">
+        <v>2</v>
+      </c>
+      <c r="H28" s="68">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="4:8" ht="15.75" customHeight="1">
+      <c r="D29" s="98"/>
+      <c r="E29" s="52" t="s">
+        <v>82</v>
+      </c>
+      <c r="F29" s="65">
+        <v>2</v>
+      </c>
+      <c r="G29" s="65">
+        <v>4</v>
+      </c>
+      <c r="H29" s="68">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="4:8">
+      <c r="D30" s="54" t="s">
         <v>58</v>
       </c>
-      <c r="H11" s="114">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="4:11">
-      <c r="D12" s="101" t="s">
-        <v>62</v>
-      </c>
-      <c r="E12" s="89" t="s">
-        <v>62</v>
-      </c>
-      <c r="F12" s="122" t="s">
-        <v>62</v>
-      </c>
-      <c r="G12" s="122" t="s">
-        <v>62</v>
-      </c>
-      <c r="H12" s="115" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="13" spans="4:11">
-      <c r="D13" s="100" t="s">
-        <v>71</v>
-      </c>
-      <c r="E13" s="86" t="s">
-        <v>72</v>
-      </c>
-      <c r="F13" s="120" t="s">
-        <v>60</v>
-      </c>
-      <c r="G13" s="120" t="s">
+      <c r="E30" s="55" t="s">
         <v>58</v>
       </c>
-      <c r="H13" s="114">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="4:11" ht="28.5" customHeight="1">
-      <c r="D14" s="100"/>
-      <c r="E14" s="86" t="s">
-        <v>73</v>
-      </c>
-      <c r="F14" s="120" t="s">
-        <v>60</v>
-      </c>
-      <c r="G14" s="120" t="s">
-        <v>61</v>
-      </c>
-      <c r="H14" s="114">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="4:11" ht="11.25" customHeight="1">
-      <c r="D15" s="100"/>
-      <c r="E15" s="86" t="s">
-        <v>74</v>
-      </c>
-      <c r="F15" s="120" t="s">
-        <v>60</v>
-      </c>
-      <c r="G15" s="120" t="s">
-        <v>57</v>
-      </c>
-      <c r="H15" s="114">
+      <c r="F30" s="73" t="s">
+        <v>58</v>
+      </c>
+      <c r="G30" s="73" t="s">
+        <v>58</v>
+      </c>
+      <c r="H30" s="69" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="4:8">
+      <c r="D31" s="57" t="s">
+        <v>83</v>
+      </c>
+      <c r="E31" s="52" t="s">
+        <v>84</v>
+      </c>
+      <c r="F31" s="65">
+        <v>1</v>
+      </c>
+      <c r="G31" s="65">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="4:11">
-      <c r="D16" s="88" t="s">
-        <v>62</v>
-      </c>
-      <c r="E16" s="89" t="s">
-        <v>62</v>
-      </c>
-      <c r="F16" s="122" t="s">
-        <v>62</v>
-      </c>
-      <c r="G16" s="122" t="s">
-        <v>62</v>
-      </c>
-      <c r="H16" s="115" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="17" spans="4:8" ht="15" customHeight="1">
-      <c r="D17" s="100" t="s">
-        <v>75</v>
-      </c>
-      <c r="E17" s="86" t="s">
-        <v>76</v>
-      </c>
-      <c r="F17" s="120" t="s">
-        <v>77</v>
-      </c>
-      <c r="G17" s="120" t="s">
-        <v>78</v>
-      </c>
-      <c r="H17" s="114">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="4:8" ht="27" customHeight="1">
-      <c r="D18" s="100"/>
-      <c r="E18" s="87" t="s">
-        <v>79</v>
-      </c>
-      <c r="F18" s="120" t="s">
-        <v>57</v>
-      </c>
-      <c r="G18" s="120" t="s">
+      <c r="H31" s="68">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="4:8">
+      <c r="D32" s="54" t="s">
         <v>58</v>
       </c>
-      <c r="H18" s="114">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="4:8" ht="27.75" customHeight="1">
-      <c r="D19" s="100"/>
-      <c r="E19" s="86" t="s">
-        <v>80</v>
-      </c>
-      <c r="F19" s="120" t="s">
+      <c r="E32" s="55" t="s">
         <v>58</v>
       </c>
-      <c r="G19" s="120" t="s">
-        <v>61</v>
-      </c>
-      <c r="H19" s="114">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="4:8">
-      <c r="D20" s="88" t="s">
-        <v>62</v>
-      </c>
-      <c r="E20" s="89" t="s">
-        <v>62</v>
-      </c>
-      <c r="F20" s="122" t="s">
-        <v>62</v>
-      </c>
-      <c r="G20" s="122" t="s">
-        <v>62</v>
-      </c>
-      <c r="H20" s="115" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="21" spans="4:8" ht="13.5" customHeight="1">
-      <c r="D21" s="118" t="s">
-        <v>81</v>
-      </c>
-      <c r="E21" s="86" t="s">
-        <v>82</v>
-      </c>
-      <c r="F21" s="120" t="s">
-        <v>57</v>
-      </c>
-      <c r="G21" s="120" t="s">
+      <c r="F32" s="55" t="s">
         <v>58</v>
       </c>
-      <c r="H21" s="114">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="4:8" ht="13.5" customHeight="1">
-      <c r="D22" s="118"/>
-      <c r="E22" s="86" t="s">
-        <v>83</v>
-      </c>
-      <c r="F22" s="120">
-        <v>2</v>
-      </c>
-      <c r="G22" s="120">
-        <v>3</v>
-      </c>
-      <c r="H22" s="114">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="4:8">
-      <c r="D23" s="118"/>
-      <c r="E23" s="87" t="s">
-        <v>84</v>
-      </c>
-      <c r="F23" s="120" t="s">
+      <c r="G32" s="55" t="s">
         <v>58</v>
       </c>
-      <c r="G23" s="120" t="s">
-        <v>78</v>
-      </c>
-      <c r="H23" s="114">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24" spans="4:8">
-      <c r="D24" s="118"/>
-      <c r="E24" s="86" t="s">
+      <c r="H32" s="56" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="33" spans="4:8">
+      <c r="D33" s="102" t="s">
         <v>85</v>
       </c>
-      <c r="F24" s="120" t="s">
-        <v>57</v>
-      </c>
-      <c r="G24" s="120" t="s">
-        <v>58</v>
-      </c>
-      <c r="H24" s="114">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="4:8">
-      <c r="D25" s="118"/>
-      <c r="E25" s="86" t="s">
-        <v>86</v>
-      </c>
-      <c r="F25" s="120" t="s">
-        <v>57</v>
-      </c>
-      <c r="G25" s="120" t="s">
-        <v>58</v>
-      </c>
-      <c r="H25" s="114">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="4:8" ht="15.75" customHeight="1">
-      <c r="D26" s="118"/>
-      <c r="E26" s="87" t="s">
-        <v>87</v>
-      </c>
-      <c r="F26" s="120" t="s">
-        <v>57</v>
-      </c>
-      <c r="G26" s="120" t="s">
-        <v>61</v>
-      </c>
-      <c r="H26" s="114">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="4:8" ht="15.75" customHeight="1">
-      <c r="D27" s="88" t="s">
-        <v>62</v>
-      </c>
-      <c r="E27" s="89" t="s">
-        <v>62</v>
-      </c>
-      <c r="F27" s="122" t="s">
-        <v>62</v>
-      </c>
-      <c r="G27" s="122" t="s">
-        <v>62</v>
-      </c>
-      <c r="H27" s="115" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="28" spans="4:8" ht="15.75" customHeight="1">
-      <c r="D28" s="105" t="s">
-        <v>88</v>
-      </c>
-      <c r="E28" s="86" t="s">
-        <v>89</v>
-      </c>
-      <c r="F28" s="120" t="s">
-        <v>57</v>
-      </c>
-      <c r="G28" s="120" t="s">
-        <v>57</v>
-      </c>
-      <c r="H28" s="114">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="4:8" ht="15.75" customHeight="1">
-      <c r="D29" s="105"/>
-      <c r="E29" s="86" t="s">
-        <v>90</v>
-      </c>
-      <c r="F29" s="120" t="s">
-        <v>57</v>
-      </c>
-      <c r="G29" s="120" t="s">
-        <v>61</v>
-      </c>
-      <c r="H29" s="114">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="30" spans="4:8">
-      <c r="D30" s="88" t="s">
-        <v>62</v>
-      </c>
-      <c r="E30" s="89" t="s">
-        <v>62</v>
-      </c>
-      <c r="F30" s="122" t="s">
-        <v>62</v>
-      </c>
-      <c r="G30" s="122" t="s">
-        <v>62</v>
-      </c>
-      <c r="H30" s="115" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="31" spans="4:8">
-      <c r="D31" s="91" t="s">
-        <v>91</v>
-      </c>
-      <c r="E31" s="86" t="s">
-        <v>92</v>
-      </c>
-      <c r="F31" s="120" t="s">
-        <v>60</v>
-      </c>
-      <c r="G31" s="120" t="s">
-        <v>57</v>
-      </c>
-      <c r="H31" s="114">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="4:8">
-      <c r="D32" s="88" t="s">
-        <v>62</v>
-      </c>
-      <c r="E32" s="89" t="s">
-        <v>62</v>
-      </c>
-      <c r="F32" s="89" t="s">
-        <v>62</v>
-      </c>
-      <c r="G32" s="89" t="s">
-        <v>62</v>
-      </c>
-      <c r="H32" s="90" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="33" spans="4:8">
-      <c r="D33" s="104" t="s">
-        <v>93</v>
-      </c>
-      <c r="E33" s="110"/>
-      <c r="F33" s="110"/>
-      <c r="G33" s="110"/>
-      <c r="H33" s="112">
+      <c r="E33" s="103"/>
+      <c r="F33" s="103"/>
+      <c r="G33" s="103"/>
+      <c r="H33" s="67">
         <f>SUM(H4:H31)</f>
         <v>149.5</v>
       </c>
     </row>
     <row r="34" spans="4:8">
-      <c r="D34" s="100" t="s">
-        <v>94</v>
-      </c>
-      <c r="E34" s="109"/>
-      <c r="F34" s="109"/>
-      <c r="G34" s="109"/>
-      <c r="H34" s="117">
-        <f>RIESGOS!J12</f>
-        <v>0.19</v>
-      </c>
-    </row>
-    <row r="35" spans="4:8" ht="30.75" customHeight="1">
-      <c r="D35" s="107" t="s">
-        <v>95</v>
-      </c>
-      <c r="E35" s="108"/>
-      <c r="F35" s="108"/>
-      <c r="G35" s="108"/>
-      <c r="H35" s="112">
-        <f>(RIESGOS!K12)</f>
-        <v>28.404999999999998</v>
+      <c r="D34" s="94" t="s">
+        <v>86</v>
+      </c>
+      <c r="E34" s="101"/>
+      <c r="F34" s="101"/>
+      <c r="G34" s="101"/>
+      <c r="H34" s="71">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="35" spans="4:8" ht="13.5" customHeight="1">
+      <c r="D35" s="99" t="s">
+        <v>87</v>
+      </c>
+      <c r="E35" s="100"/>
+      <c r="F35" s="100"/>
+      <c r="G35" s="100"/>
+      <c r="H35" s="83">
+        <f>(H33*H34)</f>
+        <v>49.335000000000001</v>
       </c>
     </row>
     <row r="36" spans="4:8">
-      <c r="D36" s="88" t="s">
-        <v>62</v>
-      </c>
-      <c r="E36" s="89" t="s">
-        <v>62</v>
-      </c>
-      <c r="F36" s="89" t="s">
-        <v>62</v>
-      </c>
-      <c r="G36" s="89" t="s">
-        <v>62</v>
-      </c>
-      <c r="H36" s="90" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="37" spans="4:8" ht="30.75" customHeight="1">
-      <c r="D37" s="107" t="s">
-        <v>96</v>
-      </c>
-      <c r="E37" s="108"/>
-      <c r="F37" s="108"/>
-      <c r="G37" s="108"/>
-      <c r="H37" s="112">
+      <c r="D36" s="54" t="s">
+        <v>58</v>
+      </c>
+      <c r="E36" s="55" t="s">
+        <v>58</v>
+      </c>
+      <c r="F36" s="55" t="s">
+        <v>58</v>
+      </c>
+      <c r="G36" s="55" t="s">
+        <v>58</v>
+      </c>
+      <c r="H36" s="56" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="37" spans="4:8" ht="12.75" customHeight="1">
+      <c r="D37" s="99" t="s">
+        <v>88</v>
+      </c>
+      <c r="E37" s="100"/>
+      <c r="F37" s="100"/>
+      <c r="G37" s="100"/>
+      <c r="H37" s="80">
         <f>(H33+H35)</f>
-        <v>177.905</v>
+        <v>198.83500000000001</v>
       </c>
     </row>
     <row r="38" spans="4:8" ht="30.75" customHeight="1">
-      <c r="D38" s="103" t="s">
-        <v>97</v>
-      </c>
-      <c r="E38" s="106"/>
-      <c r="F38" s="92" t="s">
-        <v>62</v>
-      </c>
-      <c r="G38" s="92" t="s">
-        <v>62</v>
-      </c>
-      <c r="H38" s="93" t="s">
-        <v>62</v>
+      <c r="D38" s="92" t="s">
+        <v>89</v>
+      </c>
+      <c r="E38" s="93"/>
+      <c r="F38" s="58" t="s">
+        <v>58</v>
+      </c>
+      <c r="G38" s="58" t="s">
+        <v>58</v>
+      </c>
+      <c r="H38" s="59" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="39" spans="4:8">
-      <c r="D39" s="94" t="s">
-        <v>62</v>
-      </c>
-      <c r="E39" s="95" t="s">
-        <v>98</v>
-      </c>
-      <c r="F39" s="96" t="s">
-        <v>62</v>
-      </c>
-      <c r="G39" s="95" t="s">
-        <v>99</v>
-      </c>
-      <c r="H39" s="97" t="s">
-        <v>100</v>
+      <c r="D39" s="60" t="s">
+        <v>58</v>
+      </c>
+      <c r="E39" s="61" t="s">
+        <v>90</v>
+      </c>
+      <c r="F39" s="62" t="s">
+        <v>58</v>
+      </c>
+      <c r="G39" s="61" t="s">
+        <v>91</v>
+      </c>
+      <c r="H39" s="81">
+        <f>H33/27</f>
+        <v>5.5370370370370372</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="12">
     <mergeCell ref="D38:E38"/>
     <mergeCell ref="D13:D15"/>
     <mergeCell ref="D4:D5"/>
@@ -6304,6 +6621,7 @@
     <mergeCell ref="D35:G35"/>
     <mergeCell ref="D34:G34"/>
     <mergeCell ref="D33:G33"/>
+    <mergeCell ref="D21:D26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6313,8 +6631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC971A1E-ED3D-4010-BA68-569469E882F2}">
   <dimension ref="B2:K33"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6330,64 +6648,67 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11">
-      <c r="B2" s="73" t="s">
+      <c r="B2" s="105" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" s="106"/>
+      <c r="D2" s="106"/>
+      <c r="E2" s="106"/>
+      <c r="F2" s="107" t="s">
+        <v>93</v>
+      </c>
+      <c r="G2" s="107"/>
+      <c r="H2" s="107"/>
+      <c r="I2" s="14" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" ht="20.25" customHeight="1">
+      <c r="B3" s="108" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3" s="109"/>
+      <c r="D3" s="109"/>
+      <c r="E3" s="109"/>
+      <c r="F3" s="109"/>
+      <c r="G3" s="109"/>
+      <c r="H3" s="109"/>
+      <c r="I3" s="110"/>
+    </row>
+    <row r="4" spans="2:11" ht="29.25" customHeight="1">
+      <c r="B4" s="111" t="s">
+        <v>96</v>
+      </c>
+      <c r="C4" s="111"/>
+      <c r="D4" s="111" t="s">
+        <v>97</v>
+      </c>
+      <c r="E4" s="111"/>
+      <c r="F4" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="I4" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
-      <c r="E2" s="74"/>
-      <c r="F2" s="75" t="s">
+      <c r="K4" t="s">
         <v>102</v>
       </c>
-      <c r="G2" s="75"/>
-      <c r="H2" s="75"/>
-      <c r="I2" s="14" t="s">
+    </row>
+    <row r="5" spans="2:11" ht="39" customHeight="1">
+      <c r="B5" s="117" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="3" spans="2:11" ht="20.25" customHeight="1">
-      <c r="B3" s="76" t="s">
+      <c r="C5" s="118"/>
+      <c r="D5" s="119" t="s">
         <v>104</v>
       </c>
-      <c r="C3" s="77"/>
-      <c r="D3" s="77"/>
-      <c r="E3" s="77"/>
-      <c r="F3" s="77"/>
-      <c r="G3" s="77"/>
-      <c r="H3" s="77"/>
-      <c r="I3" s="78"/>
-    </row>
-    <row r="4" spans="2:11" ht="29.25" customHeight="1">
-      <c r="B4" s="79" t="s">
-        <v>105</v>
-      </c>
-      <c r="C4" s="79"/>
-      <c r="D4" s="79" t="s">
-        <v>106</v>
-      </c>
-      <c r="E4" s="79"/>
-      <c r="F4" s="15" t="s">
-        <v>107</v>
-      </c>
-      <c r="G4" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="H4" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="I4" s="15" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" ht="39" customHeight="1">
-      <c r="B5" s="68" t="s">
-        <v>111</v>
-      </c>
-      <c r="C5" s="69"/>
-      <c r="D5" s="70" t="s">
-        <v>112</v>
-      </c>
-      <c r="E5" s="70"/>
+      <c r="E5" s="119"/>
       <c r="F5" s="8">
         <v>3</v>
       </c>
@@ -6399,25 +6720,25 @@
         <v>9</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="J5" s="111">
+        <v>105</v>
+      </c>
+      <c r="J5" s="66">
         <v>0.03</v>
       </c>
-      <c r="K5" s="116">
+      <c r="K5" s="70">
         <f>J5*ESTIMACION!$H$33</f>
         <v>4.4849999999999994</v>
       </c>
     </row>
     <row r="6" spans="2:11" ht="31.5" customHeight="1">
-      <c r="B6" s="71" t="s">
-        <v>114</v>
-      </c>
-      <c r="C6" s="70"/>
-      <c r="D6" s="72" t="s">
-        <v>115</v>
-      </c>
-      <c r="E6" s="72"/>
+      <c r="B6" s="120" t="s">
+        <v>106</v>
+      </c>
+      <c r="C6" s="119"/>
+      <c r="D6" s="121" t="s">
+        <v>107</v>
+      </c>
+      <c r="E6" s="121"/>
       <c r="F6" s="8">
         <v>3</v>
       </c>
@@ -6429,25 +6750,25 @@
         <v>9</v>
       </c>
       <c r="I6" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="J6" s="111">
+        <v>108</v>
+      </c>
+      <c r="J6" s="66">
         <v>0.03</v>
       </c>
-      <c r="K6" s="116">
+      <c r="K6" s="70">
         <f>J6*ESTIMACION!$H$33</f>
         <v>4.4849999999999994</v>
       </c>
     </row>
     <row r="7" spans="2:11" ht="40.5" customHeight="1">
-      <c r="B7" s="71" t="s">
-        <v>117</v>
-      </c>
-      <c r="C7" s="70"/>
-      <c r="D7" s="70" t="s">
-        <v>118</v>
-      </c>
-      <c r="E7" s="70"/>
+      <c r="B7" s="120" t="s">
+        <v>109</v>
+      </c>
+      <c r="C7" s="119"/>
+      <c r="D7" s="119" t="s">
+        <v>110</v>
+      </c>
+      <c r="E7" s="119"/>
       <c r="F7" s="8">
         <v>1</v>
       </c>
@@ -6459,25 +6780,25 @@
         <v>3</v>
       </c>
       <c r="I7" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="J7" s="111">
+        <v>111</v>
+      </c>
+      <c r="J7" s="66">
         <v>0.01</v>
       </c>
-      <c r="K7" s="116">
+      <c r="K7" s="70">
         <f>J7*ESTIMACION!$H$33</f>
         <v>1.4950000000000001</v>
       </c>
     </row>
     <row r="8" spans="2:11" ht="54.75" customHeight="1">
-      <c r="B8" s="71" t="s">
-        <v>120</v>
-      </c>
-      <c r="C8" s="70"/>
-      <c r="D8" s="70" t="s">
-        <v>121</v>
-      </c>
-      <c r="E8" s="70"/>
+      <c r="B8" s="120" t="s">
+        <v>112</v>
+      </c>
+      <c r="C8" s="119"/>
+      <c r="D8" s="119" t="s">
+        <v>113</v>
+      </c>
+      <c r="E8" s="119"/>
       <c r="F8" s="8">
         <v>3</v>
       </c>
@@ -6489,25 +6810,25 @@
         <v>9</v>
       </c>
       <c r="I8" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="J8" s="111">
+        <v>114</v>
+      </c>
+      <c r="J8" s="66">
         <v>0.03</v>
       </c>
-      <c r="K8" s="116">
+      <c r="K8" s="70">
         <f>J8*ESTIMACION!$H$33</f>
         <v>4.4849999999999994</v>
       </c>
     </row>
     <row r="9" spans="2:11" ht="30" customHeight="1">
-      <c r="B9" s="82" t="s">
-        <v>123</v>
-      </c>
-      <c r="C9" s="72"/>
-      <c r="D9" s="72" t="s">
-        <v>124</v>
-      </c>
-      <c r="E9" s="72"/>
+      <c r="B9" s="123" t="s">
+        <v>115</v>
+      </c>
+      <c r="C9" s="121"/>
+      <c r="D9" s="121" t="s">
+        <v>116</v>
+      </c>
+      <c r="E9" s="121"/>
       <c r="F9" s="8">
         <v>3</v>
       </c>
@@ -6519,25 +6840,25 @@
         <v>6</v>
       </c>
       <c r="I9" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="J9" s="111">
+        <v>117</v>
+      </c>
+      <c r="J9" s="66">
         <v>0.03</v>
       </c>
-      <c r="K9" s="116">
+      <c r="K9" s="70">
         <f>J9*ESTIMACION!$H$33</f>
         <v>4.4849999999999994</v>
       </c>
     </row>
     <row r="10" spans="2:11" ht="30.75" customHeight="1">
-      <c r="B10" s="82" t="s">
-        <v>126</v>
-      </c>
-      <c r="C10" s="72"/>
-      <c r="D10" s="72" t="s">
-        <v>127</v>
-      </c>
-      <c r="E10" s="72"/>
+      <c r="B10" s="123" t="s">
+        <v>118</v>
+      </c>
+      <c r="C10" s="121"/>
+      <c r="D10" s="121" t="s">
+        <v>119</v>
+      </c>
+      <c r="E10" s="121"/>
       <c r="F10" s="8">
         <v>3</v>
       </c>
@@ -6549,25 +6870,25 @@
         <v>9</v>
       </c>
       <c r="I10" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="J10" s="111">
+        <v>120</v>
+      </c>
+      <c r="J10" s="66">
         <v>0.03</v>
       </c>
-      <c r="K10" s="116">
+      <c r="K10" s="70">
         <f>J10*ESTIMACION!$H$33</f>
         <v>4.4849999999999994</v>
       </c>
     </row>
     <row r="11" spans="2:11" ht="39.75" customHeight="1">
-      <c r="B11" s="80" t="s">
-        <v>129</v>
-      </c>
-      <c r="C11" s="81"/>
-      <c r="D11" s="81" t="s">
-        <v>130</v>
-      </c>
-      <c r="E11" s="81"/>
+      <c r="B11" s="122" t="s">
+        <v>121</v>
+      </c>
+      <c r="C11" s="104"/>
+      <c r="D11" s="104" t="s">
+        <v>122</v>
+      </c>
+      <c r="E11" s="104"/>
       <c r="F11" s="11">
         <v>3</v>
       </c>
@@ -6579,69 +6900,69 @@
         <v>6</v>
       </c>
       <c r="I11" s="13" t="s">
-        <v>131</v>
-      </c>
-      <c r="J11" s="111">
+        <v>123</v>
+      </c>
+      <c r="J11" s="66">
         <v>0.03</v>
       </c>
-      <c r="K11" s="116">
+      <c r="K11" s="70">
         <f>J11*ESTIMACION!$H$33</f>
         <v>4.4849999999999994</v>
       </c>
     </row>
     <row r="12" spans="2:11">
-      <c r="J12" s="111">
+      <c r="J12" s="66">
         <f>SUM(J5:J11)</f>
         <v>0.19</v>
       </c>
-      <c r="K12" s="116">
+      <c r="K12" s="70">
         <f>SUM(K5:K11)</f>
         <v>28.404999999999998</v>
       </c>
     </row>
     <row r="13" spans="2:11">
-      <c r="B13" s="63" t="s">
-        <v>132</v>
-      </c>
-      <c r="C13" s="64"/>
-      <c r="D13" s="64"/>
-      <c r="E13" s="64"/>
-      <c r="F13" s="64"/>
-      <c r="G13" s="64"/>
-      <c r="H13" s="64"/>
-      <c r="I13" s="65"/>
+      <c r="B13" s="112" t="s">
+        <v>124</v>
+      </c>
+      <c r="C13" s="113"/>
+      <c r="D13" s="113"/>
+      <c r="E13" s="113"/>
+      <c r="F13" s="113"/>
+      <c r="G13" s="113"/>
+      <c r="H13" s="113"/>
+      <c r="I13" s="114"/>
     </row>
     <row r="14" spans="2:11" ht="28.5">
-      <c r="B14" s="66" t="s">
-        <v>105</v>
-      </c>
-      <c r="C14" s="67"/>
-      <c r="D14" s="67" t="s">
-        <v>106</v>
-      </c>
-      <c r="E14" s="67"/>
+      <c r="B14" s="115" t="s">
+        <v>96</v>
+      </c>
+      <c r="C14" s="116"/>
+      <c r="D14" s="116" t="s">
+        <v>97</v>
+      </c>
+      <c r="E14" s="116"/>
       <c r="F14" s="20" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="G14" s="20" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="H14" s="20" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="I14" s="21" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="2:11" ht="42" customHeight="1">
-      <c r="B15" s="61" t="s">
-        <v>133</v>
-      </c>
-      <c r="C15" s="59"/>
-      <c r="D15" s="59" t="s">
-        <v>134</v>
-      </c>
-      <c r="E15" s="59"/>
+      <c r="B15" s="128" t="s">
+        <v>125</v>
+      </c>
+      <c r="C15" s="126"/>
+      <c r="D15" s="126" t="s">
+        <v>126</v>
+      </c>
+      <c r="E15" s="126"/>
       <c r="F15" s="16">
         <v>2</v>
       </c>
@@ -6653,18 +6974,18 @@
         <v>6</v>
       </c>
       <c r="I15" s="22" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="16" spans="2:11" ht="42" customHeight="1">
-      <c r="B16" s="62" t="s">
-        <v>136</v>
-      </c>
-      <c r="C16" s="60"/>
-      <c r="D16" s="60" t="s">
-        <v>137</v>
-      </c>
-      <c r="E16" s="60"/>
+      <c r="B16" s="129" t="s">
+        <v>128</v>
+      </c>
+      <c r="C16" s="127"/>
+      <c r="D16" s="127" t="s">
+        <v>129</v>
+      </c>
+      <c r="E16" s="127"/>
       <c r="F16" s="18">
         <v>3</v>
       </c>
@@ -6676,18 +6997,18 @@
         <v>9</v>
       </c>
       <c r="I16" s="23" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
     </row>
     <row r="17" spans="2:9" ht="47.25" customHeight="1">
-      <c r="B17" s="62" t="s">
-        <v>139</v>
-      </c>
-      <c r="C17" s="60"/>
-      <c r="D17" s="60" t="s">
-        <v>140</v>
-      </c>
-      <c r="E17" s="60"/>
+      <c r="B17" s="129" t="s">
+        <v>131</v>
+      </c>
+      <c r="C17" s="127"/>
+      <c r="D17" s="127" t="s">
+        <v>132</v>
+      </c>
+      <c r="E17" s="127"/>
       <c r="F17" s="18">
         <v>3</v>
       </c>
@@ -6699,18 +7020,18 @@
         <v>6</v>
       </c>
       <c r="I17" s="23" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
     </row>
     <row r="18" spans="2:9" ht="51" customHeight="1">
-      <c r="B18" s="62" t="s">
-        <v>142</v>
-      </c>
-      <c r="C18" s="60"/>
-      <c r="D18" s="60" t="s">
-        <v>143</v>
-      </c>
-      <c r="E18" s="60"/>
+      <c r="B18" s="129" t="s">
+        <v>134</v>
+      </c>
+      <c r="C18" s="127"/>
+      <c r="D18" s="127" t="s">
+        <v>135</v>
+      </c>
+      <c r="E18" s="127"/>
       <c r="F18" s="18">
         <v>3</v>
       </c>
@@ -6722,18 +7043,18 @@
         <v>6</v>
       </c>
       <c r="I18" s="23" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
     </row>
     <row r="19" spans="2:9" ht="42.75" customHeight="1">
-      <c r="B19" s="62" t="s">
-        <v>145</v>
-      </c>
-      <c r="C19" s="60"/>
-      <c r="D19" s="60" t="s">
-        <v>146</v>
-      </c>
-      <c r="E19" s="60"/>
+      <c r="B19" s="129" t="s">
+        <v>137</v>
+      </c>
+      <c r="C19" s="127"/>
+      <c r="D19" s="127" t="s">
+        <v>138</v>
+      </c>
+      <c r="E19" s="127"/>
       <c r="F19" s="18">
         <v>2</v>
       </c>
@@ -6745,18 +7066,18 @@
         <v>6</v>
       </c>
       <c r="I19" s="23" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
     </row>
     <row r="20" spans="2:9" ht="43.5" customHeight="1">
-      <c r="B20" s="57" t="s">
-        <v>148</v>
-      </c>
-      <c r="C20" s="58"/>
-      <c r="D20" s="58" t="s">
-        <v>149</v>
-      </c>
-      <c r="E20" s="58"/>
+      <c r="B20" s="124" t="s">
+        <v>140</v>
+      </c>
+      <c r="C20" s="125"/>
+      <c r="D20" s="125" t="s">
+        <v>141</v>
+      </c>
+      <c r="E20" s="125"/>
       <c r="F20" s="19">
         <v>2</v>
       </c>
@@ -6768,7 +7089,7 @@
         <v>4</v>
       </c>
       <c r="I20" s="24" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
     </row>
     <row r="21" spans="2:9">
@@ -6776,19 +7097,22 @@
       <c r="C21" s="1"/>
     </row>
     <row r="33" spans="8:8">
-      <c r="H33" s="111">
-        <f>(RIESGOS!J12)</f>
-        <v>0.19</v>
-      </c>
+      <c r="H33" s="66"/>
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="B3:I3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
     <mergeCell ref="B13:I13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="D14:E14"/>
@@ -6805,18 +7129,12 @@
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="B3:I3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:E4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6824,80 +7142,154 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCBCABF7-6294-4DBF-A467-DEA8A8CAED00}">
-  <dimension ref="B2:E5"/>
+  <dimension ref="A2:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:E5"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col min="1" max="1" width="20.85546875" customWidth="1"/>
     <col min="2" max="2" width="15.42578125" customWidth="1"/>
     <col min="3" max="3" width="34.5703125" customWidth="1"/>
     <col min="4" max="4" width="29.42578125" customWidth="1"/>
     <col min="5" max="5" width="31.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5">
+    <row r="2" spans="1:5">
       <c r="B2" s="33" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="C2" s="34" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="D2" s="34" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E2" s="35" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="3" spans="2:5" ht="72">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="72">
       <c r="B3" s="27">
         <v>1</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="E3" s="28" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" ht="115.5">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="115.5">
       <c r="B4" s="27">
         <v>2</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="D4" s="26" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="E4" s="28" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" ht="129.75">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="129.75">
       <c r="B5" s="29">
         <v>3</v>
       </c>
       <c r="C5" s="30" t="s">
+        <v>153</v>
+      </c>
+      <c r="D5" s="31" t="s">
+        <v>154</v>
+      </c>
+      <c r="E5" s="32" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="133" t="s">
+        <v>156</v>
+      </c>
+      <c r="B8" s="133"/>
+      <c r="C8" s="133"/>
+      <c r="D8" s="133"/>
+      <c r="E8" s="130"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="131"/>
+      <c r="B9" s="134" t="s">
+        <v>157</v>
+      </c>
+      <c r="C9" s="135" t="s">
+        <v>158</v>
+      </c>
+      <c r="D9" s="135" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="136" t="s">
+        <v>160</v>
+      </c>
+      <c r="B10" s="132"/>
+      <c r="C10" s="131"/>
+      <c r="D10" s="131"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="136" t="s">
         <v>161</v>
       </c>
-      <c r="D5" s="31" t="s">
+      <c r="B11" s="132"/>
+      <c r="C11" s="131"/>
+      <c r="D11" s="131"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="136" t="s">
         <v>162</v>
       </c>
-      <c r="E5" s="32" t="s">
+      <c r="B12" s="131"/>
+      <c r="C12" s="132"/>
+      <c r="D12" s="131"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="136" t="s">
         <v>163</v>
       </c>
+      <c r="B13" s="132"/>
+      <c r="C13" s="132"/>
+      <c r="D13" s="131"/>
+    </row>
+    <row r="14" spans="1:5" ht="28.5">
+      <c r="A14" s="137" t="s">
+        <v>164</v>
+      </c>
+      <c r="B14" s="132"/>
+      <c r="C14" s="131"/>
+      <c r="D14" s="131"/>
+    </row>
+    <row r="15" spans="1:5" ht="28.5">
+      <c r="A15" s="138" t="s">
+        <v>165</v>
+      </c>
+      <c r="B15" s="132"/>
+      <c r="C15" s="131"/>
+      <c r="D15" s="131"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A8:D8"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -6906,7 +7298,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58D9BC44-7C49-4BD4-811C-DAECB2CEE96F}">
   <dimension ref="B2:O10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -6931,296 +7323,296 @@
   <sheetData>
     <row r="2" spans="2:15" ht="18.75" customHeight="1">
       <c r="B2" s="36" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="C2" s="37" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="E2" s="36" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="F2" s="37" t="s">
+        <v>168</v>
+      </c>
+      <c r="H2" s="36" t="s">
         <v>166</v>
       </c>
-      <c r="H2" s="36" t="s">
-        <v>164</v>
-      </c>
       <c r="I2" s="37" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="K2" s="36" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="L2" s="37" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="N2" s="36" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="O2" s="37" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="3" spans="2:15" ht="30.75" customHeight="1">
       <c r="B3" s="36" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C3" s="42" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="E3" s="36" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="F3" s="39" t="s">
+        <v>174</v>
+      </c>
+      <c r="H3" s="36" t="s">
         <v>172</v>
       </c>
-      <c r="H3" s="36" t="s">
-        <v>170</v>
-      </c>
       <c r="I3" s="39" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="K3" s="36" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="L3" s="39" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="N3" s="36" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="O3" s="39" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
     </row>
     <row r="4" spans="2:15" ht="15.75" customHeight="1">
       <c r="B4" s="36" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C4" s="42" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="E4" s="36" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="F4" s="38" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="H4" s="36" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="I4" s="38" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="K4" s="36" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="L4" s="38" t="s">
+        <v>180</v>
+      </c>
+      <c r="N4" s="36" t="s">
         <v>178</v>
       </c>
-      <c r="N4" s="36" t="s">
-        <v>176</v>
-      </c>
       <c r="O4" s="38" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5" spans="2:15" ht="20.25" customHeight="1">
       <c r="B5" s="36" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C5" s="42" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="E5" s="36" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="F5" s="38" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="H5" s="36" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="I5" s="38" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="K5" s="36" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="L5" s="38" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="N5" s="36" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="O5" s="38" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="6" spans="2:15" ht="126" customHeight="1">
       <c r="B6" s="36" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C6" s="40" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="E6" s="36" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="F6" s="44" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="H6" s="36" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="I6" s="44" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="K6" s="36" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="L6" s="44" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="N6" s="36" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="O6" s="44" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="7" spans="2:15" ht="36.75" customHeight="1">
       <c r="B7" s="36" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C7" s="43" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="E7" s="36" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="F7" s="40" t="s">
+        <v>188</v>
+      </c>
+      <c r="H7" s="36" t="s">
         <v>186</v>
       </c>
-      <c r="H7" s="36" t="s">
-        <v>184</v>
-      </c>
       <c r="I7" s="40" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="K7" s="36" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="L7" s="40" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="N7" s="36" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="O7" s="40" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="8" spans="2:15" ht="123" customHeight="1">
       <c r="B8" s="36" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C8" s="43" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="E8" s="36" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F8" s="40" t="s">
+        <v>193</v>
+      </c>
+      <c r="H8" s="36" t="s">
         <v>191</v>
       </c>
-      <c r="H8" s="36" t="s">
-        <v>189</v>
-      </c>
       <c r="I8" s="40" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="K8" s="36" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="L8" s="40" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="N8" s="36" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="O8" s="40" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
     <row r="9" spans="2:15" ht="156" customHeight="1">
       <c r="B9" s="36" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="C9" s="43" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="E9" s="36" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="F9" s="43" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="36" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="I9" s="43" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="J9" s="1"/>
       <c r="K9" s="36" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="L9" s="43" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="M9" s="1"/>
       <c r="N9" s="36" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="O9" s="43" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row r="10" spans="2:15" ht="157.5" customHeight="1">
       <c r="B10" s="36" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="C10" s="43" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="E10" s="36" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="F10" s="40" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="36" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="I10" s="40" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="J10" s="1"/>
       <c r="K10" s="36" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="L10" s="40" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="M10" s="1"/>
       <c r="N10" s="36" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="O10" s="40" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -7251,242 +7643,242 @@
     <row r="2" spans="2:9" ht="6" customHeight="1"/>
     <row r="3" spans="2:9">
       <c r="B3" s="36" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="C3" s="37" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="E3" s="36" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="F3" s="37" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="H3" s="36" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="I3" s="37" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="4" spans="2:9" ht="89.25" customHeight="1">
       <c r="B4" s="36" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C4" s="43" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="E4" s="36" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="F4" s="43" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="H4" s="36" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="I4" s="43" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="5" spans="2:9">
       <c r="B5" s="36" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C5" s="42" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="E5" s="36" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="F5" s="42" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="H5" s="36" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="I5" s="42" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="6" spans="2:9">
       <c r="B6" s="36" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C6" s="42" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="E6" s="36" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="F6" s="42" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="H6" s="36" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="I6" s="42" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="7" spans="2:9" ht="150" customHeight="1">
       <c r="B7" s="36" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C7" s="43" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="E7" s="36" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F7" s="43" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="H7" s="36" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="I7" s="43" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="8" spans="2:9" ht="72" customHeight="1">
       <c r="B8" s="36" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="C8" s="43" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="E8" s="36" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="F8" s="43" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="H8" s="36" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="I8" s="43" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
     <row r="10" spans="2:9">
       <c r="B10" s="36" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="C10" s="37" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="E10" s="36" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="F10" s="37" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="H10" s="36" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="I10" s="37" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
     </row>
     <row r="11" spans="2:9" ht="68.25" customHeight="1">
       <c r="B11" s="36" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C11" s="43" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="E11" s="36" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="F11" s="43" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="H11" s="36" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="I11" s="43" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
     <row r="12" spans="2:9">
       <c r="B12" s="36" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C12" s="42" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="E12" s="36" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="F12" s="42" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="H12" s="36" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="I12" s="42" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="13" spans="2:9">
       <c r="B13" s="36" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C13" s="42" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="E13" s="36" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="F13" s="42" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="H13" s="36" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="I13" s="42" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="14" spans="2:9" ht="171" customHeight="1">
       <c r="B14" s="36" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C14" s="43" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="E14" s="36" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F14" s="43" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="H14" s="36" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="I14" s="43" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="15" spans="2:9" ht="45.75">
       <c r="B15" s="36" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="C15" s="43" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="E15" s="36" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="F15" s="43" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="H15" s="36" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="I15" s="43" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
     </row>
   </sheetData>
@@ -7518,82 +7910,82 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:13" ht="18">
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
-      <c r="L2" s="84"/>
-      <c r="M2" s="84"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="50"/>
+      <c r="K2" s="50"/>
+      <c r="L2" s="50"/>
+      <c r="M2" s="50"/>
     </row>
     <row r="3" spans="2:13" ht="57.75" customHeight="1">
       <c r="B3" s="45" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="C3" s="45" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="D3" s="45" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="E3" s="45" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="F3" s="45" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="G3" s="45" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="H3" s="45" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="I3" s="45" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="J3" s="47" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="K3" s="45" t="s">
-        <v>239</v>
-      </c>
-      <c r="L3" s="83"/>
+        <v>241</v>
+      </c>
+      <c r="L3" s="49"/>
     </row>
     <row r="4" spans="2:13" ht="91.5">
       <c r="B4" s="41">
         <v>1</v>
       </c>
       <c r="C4" s="41" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="D4" s="43" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="E4" s="41" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="F4" s="46">
         <v>44979</v>
       </c>
       <c r="G4" s="41" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="H4" s="41" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="I4" s="41" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="J4" s="41" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="K4" s="48" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="5" spans="2:13" ht="76.5">
@@ -7601,31 +7993,31 @@
         <v>2</v>
       </c>
       <c r="C5" s="41" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="D5" s="43" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="E5" s="41" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="F5" s="46">
         <v>44979</v>
       </c>
       <c r="G5" s="41" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="H5" s="41" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="I5" s="41" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="J5" s="41" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="K5" s="41" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
   </sheetData>

</xml_diff>